<commit_message>
Do some part of importing study program
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1D2402-9D3E-4683-AC67-5ED29E90C562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B10DE39-797B-454C-85FF-8D6BE861862A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -1690,9 +1690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE44191-4F7D-454A-9855-FE690642DDD6}">
   <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N1" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5470,6 +5470,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A95A7398140C45A2F719D38434B23A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8f464c4684f4805cd2f27ee87272a526">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07db5020-ba8e-48bf-aa17-fbace2a70736" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1a8c984c74c8b52243a5f41979946bd" ns2:_="">
     <xsd:import namespace="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
@@ -5617,15 +5626,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{179DDC9E-E391-4AD2-A488-D9C201286EF9}">
   <ds:schemaRefs>
@@ -5637,6 +5637,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648878AA-48B2-4081-A1D0-3EB795A895EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5652,12 +5660,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Validation for Import study program
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B10DE39-797B-454C-85FF-8D6BE861862A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D987870C-B0C2-472B-AB35-6A05816F884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -1690,9 +1690,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE44191-4F7D-454A-9855-FE690642DDD6}">
   <dimension ref="A1:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Import successfully (only main flow)
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D987870C-B0C2-472B-AB35-6A05816F884C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5857406A-63FB-4054-A099-F7984C8E97CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="280">
   <si>
     <t>STT</t>
   </si>
@@ -1688,11 +1688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE44191-4F7D-454A-9855-FE690642DDD6}">
-  <dimension ref="A1:S87"/>
+  <dimension ref="A1:S85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4700,40 +4700,36 @@
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
-        <v>70</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="E71" s="5">
-        <v>3</v>
-      </c>
-      <c r="F71" s="5">
-        <v>30</v>
-      </c>
-      <c r="G71" s="5">
-        <v>30</v>
-      </c>
-      <c r="H71" s="5">
-        <v>0</v>
-      </c>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D71" s="6"/>
+      <c r="E71" s="7">
+        <v>3</v>
+      </c>
+      <c r="F71" s="7">
+        <v>30</v>
+      </c>
+      <c r="G71" s="7">
+        <v>30</v>
+      </c>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K71" s="5" t="s">
+      <c r="K71" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L71" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M71" s="4"/>
+      <c r="L71" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="M71" s="6"/>
       <c r="N71" s="30" t="s">
         <v>267</v>
       </c>
@@ -4743,16 +4739,16 @@
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="E72" s="5">
         <v>3</v>
@@ -4786,36 +4782,40 @@
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
-        <v>72</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D73" s="6"/>
-      <c r="E73" s="7">
-        <v>3</v>
-      </c>
-      <c r="F73" s="7">
-        <v>30</v>
-      </c>
-      <c r="G73" s="7">
-        <v>30</v>
-      </c>
-      <c r="H73" s="7"/>
-      <c r="I73" s="7"/>
-      <c r="J73" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E73" s="5">
+        <v>3</v>
+      </c>
+      <c r="F73" s="5">
+        <v>0</v>
+      </c>
+      <c r="G73" s="5">
+        <v>0</v>
+      </c>
+      <c r="H73" s="5">
+        <v>0</v>
+      </c>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K73" s="7" t="s">
+      <c r="K73" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L73" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="M73" s="6"/>
+      <c r="L73" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M73" s="4"/>
       <c r="N73" s="30" t="s">
         <v>267</v>
       </c>
@@ -4825,16 +4825,16 @@
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E74" s="5">
         <v>3</v>
@@ -4868,16 +4868,16 @@
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="E75" s="5">
         <v>3</v>
@@ -4911,25 +4911,25 @@
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="E76" s="5">
         <v>3</v>
       </c>
       <c r="F76" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G76" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H76" s="5">
         <v>0</v>
@@ -4952,70 +4952,74 @@
         <v>277</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>76</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="E77" s="5">
-        <v>3</v>
-      </c>
-      <c r="F77" s="5">
-        <v>0</v>
-      </c>
-      <c r="G77" s="5">
-        <v>0</v>
-      </c>
-      <c r="H77" s="5">
-        <v>0</v>
-      </c>
-      <c r="I77" s="5"/>
-      <c r="J77" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="E77" s="13">
+        <v>3</v>
+      </c>
+      <c r="F77" s="13">
+        <v>30</v>
+      </c>
+      <c r="G77" s="13">
+        <v>30</v>
+      </c>
+      <c r="H77" s="13">
+        <v>0</v>
+      </c>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K77" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L77" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M77" s="4"/>
+      <c r="K77" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L77" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="M77" s="18"/>
       <c r="N77" s="30" t="s">
         <v>267</v>
       </c>
       <c r="O77" s="37" t="s">
         <v>277</v>
       </c>
+      <c r="P77" s="14"/>
+      <c r="Q77" s="14"/>
+      <c r="R77" s="14"/>
+      <c r="S77" s="14"/>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
-        <v>77</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>221</v>
+        <v>79</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>238</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="E78" s="5">
         <v>3</v>
       </c>
       <c r="F78" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G78" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H78" s="5">
         <v>0</v>
@@ -5025,12 +5029,12 @@
         <v>4</v>
       </c>
       <c r="K78" s="5" t="s">
-        <v>16</v>
+        <v>189</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M78" s="4"/>
+        <v>125</v>
+      </c>
+      <c r="M78" s="18"/>
       <c r="N78" s="30" t="s">
         <v>267</v>
       </c>
@@ -5038,39 +5042,39 @@
         <v>277</v>
       </c>
     </row>
-    <row r="79" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="E79" s="13">
-        <v>3</v>
-      </c>
-      <c r="F79" s="13">
-        <v>30</v>
-      </c>
-      <c r="G79" s="13">
-        <v>30</v>
-      </c>
-      <c r="H79" s="13">
-        <v>0</v>
-      </c>
-      <c r="I79" s="13"/>
-      <c r="J79" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E79" s="5">
+        <v>3</v>
+      </c>
+      <c r="F79" s="5">
+        <v>30</v>
+      </c>
+      <c r="G79" s="5">
+        <v>30</v>
+      </c>
+      <c r="H79" s="5">
+        <v>0</v>
+      </c>
+      <c r="I79" s="5"/>
+      <c r="J79" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K79" s="13" t="s">
+      <c r="K79" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L79" s="18" t="s">
+      <c r="L79" s="4" t="s">
         <v>110</v>
       </c>
       <c r="M79" s="18"/>
@@ -5080,45 +5084,41 @@
       <c r="O79" s="37" t="s">
         <v>277</v>
       </c>
-      <c r="P79" s="14"/>
-      <c r="Q79" s="14"/>
-      <c r="R79" s="14"/>
-      <c r="S79" s="14"/>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="E80" s="5">
-        <v>3</v>
-      </c>
-      <c r="F80" s="5">
-        <v>30</v>
-      </c>
-      <c r="G80" s="5">
-        <v>30</v>
-      </c>
-      <c r="H80" s="5">
-        <v>0</v>
-      </c>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E80" s="13">
+        <v>3</v>
+      </c>
+      <c r="F80" s="13">
+        <v>30</v>
+      </c>
+      <c r="G80" s="13">
+        <v>30</v>
+      </c>
+      <c r="H80" s="13">
+        <v>0</v>
+      </c>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K80" s="5" t="s">
-        <v>189</v>
+      <c r="K80" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="M80" s="18"/>
       <c r="N80" s="30" t="s">
@@ -5127,19 +5127,23 @@
       <c r="O80" s="37" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P80" s="14"/>
+      <c r="Q80" s="14"/>
+      <c r="R80" s="14"/>
+      <c r="S80" s="14"/>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="E81" s="5">
         <v>3</v>
@@ -5158,7 +5162,7 @@
         <v>4</v>
       </c>
       <c r="K81" s="5" t="s">
-        <v>68</v>
+        <v>189</v>
       </c>
       <c r="L81" s="4" t="s">
         <v>110</v>
@@ -5171,239 +5175,149 @@
         <v>277</v>
       </c>
     </row>
-    <row r="82" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
-        <v>81</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="C82" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="D82" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="E82" s="13">
-        <v>3</v>
-      </c>
-      <c r="F82" s="13">
-        <v>30</v>
-      </c>
-      <c r="G82" s="13">
-        <v>30</v>
-      </c>
-      <c r="H82" s="13">
-        <v>0</v>
-      </c>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K82" s="13" t="s">
-        <v>68</v>
+        <v>83</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E82" s="5">
+        <v>2</v>
+      </c>
+      <c r="F82" s="5">
+        <v>0</v>
+      </c>
+      <c r="G82" s="5">
+        <v>0</v>
+      </c>
+      <c r="H82" s="5">
+        <v>60</v>
+      </c>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K82" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M82" s="18"/>
+        <v>16</v>
+      </c>
+      <c r="M82" s="4"/>
       <c r="N82" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="O82" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="P82" s="14"/>
-      <c r="Q82" s="14"/>
-      <c r="R82" s="14"/>
-      <c r="S82" s="14"/>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="O82" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
-        <v>82</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>247</v>
+        <v>84</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>254</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="E83" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F83" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G83" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H83" s="5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="I83" s="5"/>
       <c r="J83" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K83" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L83" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="M83" s="4"/>
+      <c r="N83" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="O83" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="20">
+        <v>85</v>
+      </c>
+      <c r="B84" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C84" s="40" t="s">
+        <v>259</v>
+      </c>
+      <c r="D84" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E84" s="41">
+        <v>6</v>
+      </c>
+      <c r="F84" s="41">
+        <v>0</v>
+      </c>
+      <c r="G84" s="41">
+        <v>0</v>
+      </c>
+      <c r="H84" s="41"/>
+      <c r="I84" s="41">
+        <v>180</v>
+      </c>
+      <c r="J84" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K83" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="L83" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M83" s="18"/>
-      <c r="N83" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="O83" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="84" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A84" s="3">
-        <v>83</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C84" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="E84" s="5">
-        <v>2</v>
-      </c>
-      <c r="F84" s="5">
-        <v>0</v>
-      </c>
-      <c r="G84" s="5">
-        <v>0</v>
-      </c>
-      <c r="H84" s="5">
-        <v>60</v>
-      </c>
-      <c r="I84" s="5"/>
-      <c r="J84" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K84" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="L84" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M84" s="4"/>
-      <c r="N84" s="30" t="s">
+      <c r="K84" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="L84" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="M84" s="40"/>
+      <c r="N84" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="O84" s="38" t="s">
+      <c r="O84" s="39" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="85" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="3">
-        <v>84</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E85" s="5">
-        <v>2</v>
-      </c>
-      <c r="F85" s="5">
-        <v>0</v>
-      </c>
-      <c r="G85" s="5">
-        <v>0</v>
-      </c>
-      <c r="H85" s="5">
-        <v>60</v>
-      </c>
-      <c r="I85" s="5"/>
-      <c r="J85" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K85" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L85" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="M85" s="4"/>
-      <c r="N85" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="O85" s="38" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="86" spans="1:19" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="20">
-        <v>85</v>
-      </c>
-      <c r="B86" s="40" t="s">
-        <v>258</v>
-      </c>
-      <c r="C86" s="40" t="s">
-        <v>259</v>
-      </c>
-      <c r="D86" s="40" t="s">
-        <v>260</v>
-      </c>
-      <c r="E86" s="41">
-        <v>6</v>
-      </c>
-      <c r="F86" s="41">
-        <v>0</v>
-      </c>
-      <c r="G86" s="41">
-        <v>0</v>
-      </c>
-      <c r="H86" s="41"/>
-      <c r="I86" s="41">
-        <v>180</v>
-      </c>
-      <c r="J86" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="K86" s="42" t="s">
-        <v>261</v>
-      </c>
-      <c r="L86" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="M86" s="40"/>
-      <c r="N86" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="O86" s="39" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A87" s="21"/>
-      <c r="B87" s="22"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="21"/>
-      <c r="H87" s="21"/>
-      <c r="I87" s="21"/>
-      <c r="J87" s="21"/>
-      <c r="K87" s="21"/>
-      <c r="L87" s="22"/>
-      <c r="M87" s="22"/>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A85" s="21"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="21"/>
+      <c r="F85" s="21"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="21"/>
+      <c r="I85" s="21"/>
+      <c r="J85" s="21"/>
+      <c r="K85" s="21"/>
+      <c r="L85" s="22"/>
+      <c r="M85" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L50">
@@ -5421,22 +5335,22 @@
       <formula>$K46&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:M47 B73:K73 M73 B74:M86 B48:M72 B2:M45 N2:O86">
+  <conditionalFormatting sqref="K46:M47 B71:K71 M71 B72:M84 B48:M70 B2:M45 N2:O84">
     <cfRule type="expression" dxfId="5" priority="5">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48:C86 B2:C45">
+  <conditionalFormatting sqref="B2:C45 B48:C84">
     <cfRule type="expression" dxfId="4" priority="6">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L70 L67 B61:B65 B79:B83">
+  <conditionalFormatting sqref="L70 L67 B61:B65 B77:B81">
     <cfRule type="expression" dxfId="3" priority="7">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L50 L73 L53">
+  <conditionalFormatting sqref="L50 L71 L53">
     <cfRule type="expression" dxfId="2" priority="8">
       <formula>#REF!&gt;=1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update database modal again
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DC8207-6003-4C53-BF86-1E7BEB2972D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BA1C99-3508-40C1-B595-AC7E683E2807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="281">
   <si>
     <t>STT</t>
   </si>
@@ -857,6 +857,9 @@
     <t>Tên loại kiến thức</t>
   </si>
   <si>
+    <t>Mã loại kiến thức</t>
+  </si>
+  <si>
     <t>Đại cương</t>
   </si>
   <si>
@@ -869,6 +872,9 @@
     <t>Cơ sở ngành</t>
   </si>
   <si>
+    <t>Chuyên ngành</t>
+  </si>
+  <si>
     <t>Chuyên ngành Công nghệ Phần mềm</t>
   </si>
   <si>
@@ -882,9 +888,6 @@
   </si>
   <si>
     <t>Thực tập tốt nghiệp/Khóa luận - Đồ án tốt nghiệp/Học phần tốt nghiệp</t>
-  </si>
-  <si>
-    <t>Mã loại kiến thức</t>
   </si>
 </sst>
 </file>
@@ -930,7 +933,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -940,6 +943,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1157,6 +1166,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1172,11 +1185,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1193,27 +1209,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF0070C0"/>
@@ -1688,11 +1707,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE44191-4F7D-454A-9855-FE690642DDD6}">
-  <dimension ref="A1:S85"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1708,54 +1727,54 @@
     <col min="12" max="12" width="23.33203125" customWidth="1"/>
     <col min="13" max="13" width="24.21875" customWidth="1"/>
     <col min="14" max="14" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.6640625" style="2" customWidth="1"/>
-    <col min="16" max="19" width="8.88671875" style="2"/>
+    <col min="15" max="15" width="33.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33" t="s">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="33" t="s">
+      <c r="D1" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="O1" s="39" t="s">
         <v>269</v>
       </c>
     </row>
@@ -1793,11 +1812,11 @@
         <v>16</v>
       </c>
       <c r="M2" s="4"/>
-      <c r="N2" s="30" t="s">
+      <c r="N2" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O2" s="37" t="s">
-        <v>270</v>
+      <c r="O2" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1834,11 +1853,11 @@
         <v>12</v>
       </c>
       <c r="M3" s="4"/>
-      <c r="N3" s="30" t="s">
+      <c r="N3" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O3" s="37" t="s">
-        <v>270</v>
+      <c r="O3" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1875,11 +1894,11 @@
         <v>12</v>
       </c>
       <c r="M4" s="4"/>
-      <c r="N4" s="30" t="s">
+      <c r="N4" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O4" s="37" t="s">
-        <v>270</v>
+      <c r="O4" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1916,11 +1935,11 @@
         <v>17</v>
       </c>
       <c r="M5" s="4"/>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O5" s="37" t="s">
-        <v>270</v>
+      <c r="O5" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1957,11 +1976,11 @@
         <v>25</v>
       </c>
       <c r="M6" s="4"/>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O6" s="37" t="s">
-        <v>270</v>
+      <c r="O6" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
@@ -1995,14 +2014,14 @@
         <v>28</v>
       </c>
       <c r="L7" s="18"/>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="30" t="s">
+      <c r="N7" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O7" s="37" t="s">
-        <v>270</v>
+      <c r="O7" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2037,11 +2056,11 @@
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="30" t="s">
+      <c r="N8" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O8" s="37" t="s">
-        <v>270</v>
+      <c r="O8" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2076,11 +2095,11 @@
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="30" t="s">
+      <c r="N9" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O9" s="37" t="s">
-        <v>270</v>
+      <c r="O9" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2115,11 +2134,11 @@
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="30" t="s">
+      <c r="N10" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O10" s="37" t="s">
-        <v>270</v>
+      <c r="O10" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2154,11 +2173,11 @@
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="30" t="s">
+      <c r="N11" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O11" s="37" t="s">
-        <v>270</v>
+      <c r="O11" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2193,11 +2212,11 @@
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O12" s="37" t="s">
-        <v>270</v>
+      <c r="O12" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2232,11 +2251,11 @@
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="30" t="s">
+      <c r="N13" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O13" s="37" t="s">
-        <v>270</v>
+      <c r="O13" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2273,11 +2292,11 @@
         <v>50</v>
       </c>
       <c r="M14" s="4"/>
-      <c r="N14" s="30" t="s">
+      <c r="N14" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O14" s="37" t="s">
-        <v>270</v>
+      <c r="O14" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2314,11 +2333,11 @@
         <v>50</v>
       </c>
       <c r="M15" s="4"/>
-      <c r="N15" s="30" t="s">
+      <c r="N15" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O15" s="37" t="s">
-        <v>270</v>
+      <c r="O15" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -2357,11 +2376,11 @@
         <v>50</v>
       </c>
       <c r="M16" s="4"/>
-      <c r="N16" s="30" t="s">
+      <c r="N16" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O16" s="37" t="s">
-        <v>270</v>
+      <c r="O16" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2400,11 +2419,11 @@
         <v>50</v>
       </c>
       <c r="M17" s="6"/>
-      <c r="N17" s="30" t="s">
+      <c r="N17" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O17" s="37" t="s">
-        <v>270</v>
+      <c r="O17" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2443,11 +2462,11 @@
         <v>50</v>
       </c>
       <c r="M18" s="4"/>
-      <c r="N18" s="30" t="s">
+      <c r="N18" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O18" s="37" t="s">
-        <v>270</v>
+      <c r="O18" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2486,11 +2505,11 @@
         <v>15</v>
       </c>
       <c r="M19" s="6"/>
-      <c r="N19" s="30" t="s">
+      <c r="N19" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O19" s="37" t="s">
-        <v>270</v>
+      <c r="O19" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2529,11 +2548,11 @@
         <v>68</v>
       </c>
       <c r="M20" s="4"/>
-      <c r="N20" s="30" t="s">
+      <c r="N20" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O20" s="37" t="s">
-        <v>270</v>
+      <c r="O20" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2572,11 +2591,11 @@
         <v>68</v>
       </c>
       <c r="M21" s="4"/>
-      <c r="N21" s="30" t="s">
+      <c r="N21" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O21" s="37" t="s">
-        <v>270</v>
+      <c r="O21" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -2615,11 +2634,11 @@
         <v>50</v>
       </c>
       <c r="M22" s="4"/>
-      <c r="N22" s="30" t="s">
+      <c r="N22" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O22" s="37" t="s">
-        <v>270</v>
+      <c r="O22" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2658,11 +2677,11 @@
         <v>50</v>
       </c>
       <c r="M23" s="4"/>
-      <c r="N23" s="30" t="s">
+      <c r="N23" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O23" s="37" t="s">
-        <v>270</v>
+      <c r="O23" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2701,11 +2720,11 @@
         <v>50</v>
       </c>
       <c r="M24" s="4"/>
-      <c r="N24" s="30" t="s">
+      <c r="N24" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O24" s="37" t="s">
-        <v>270</v>
+      <c r="O24" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2744,253 +2763,253 @@
         <v>50</v>
       </c>
       <c r="M25" s="4"/>
-      <c r="N25" s="30" t="s">
+      <c r="N25" s="32" t="s">
         <v>262</v>
       </c>
-      <c r="O25" s="37" t="s">
-        <v>270</v>
+      <c r="O25" s="40" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="32">
+      <c r="A26" s="35">
         <v>25</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="26">
+      <c r="D26" s="27"/>
+      <c r="E26" s="28">
         <v>2</v>
       </c>
-      <c r="F26" s="27">
-        <v>0</v>
-      </c>
-      <c r="G26" s="27">
+      <c r="F26" s="29">
+        <v>0</v>
+      </c>
+      <c r="G26" s="29">
         <v>60</v>
       </c>
-      <c r="H26" s="27">
-        <v>0</v>
-      </c>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27" t="s">
+      <c r="H26" s="29">
+        <v>0</v>
+      </c>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="K26" s="27" t="s">
+      <c r="K26" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="L26" s="25" t="s">
+      <c r="L26" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="M26" s="25"/>
-      <c r="N26" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="O26" s="38" t="s">
+      <c r="M26" s="27"/>
+      <c r="N26" s="32" t="s">
         <v>272</v>
       </c>
+      <c r="O26" s="40" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="32">
+      <c r="A27" s="35">
         <v>26</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="26">
+      <c r="D27" s="27"/>
+      <c r="E27" s="28">
         <v>2</v>
       </c>
-      <c r="F27" s="27">
-        <v>0</v>
-      </c>
-      <c r="G27" s="27">
+      <c r="F27" s="29">
+        <v>0</v>
+      </c>
+      <c r="G27" s="29">
         <v>60</v>
       </c>
-      <c r="H27" s="27">
-        <v>0</v>
-      </c>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27" t="s">
+      <c r="H27" s="29">
+        <v>0</v>
+      </c>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="K27" s="27" t="s">
+      <c r="K27" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="L27" s="25" t="s">
+      <c r="L27" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="M27" s="25"/>
-      <c r="N27" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="O27" s="38" t="s">
+      <c r="M27" s="27"/>
+      <c r="N27" s="32" t="s">
         <v>272</v>
       </c>
+      <c r="O27" s="40" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="32">
+      <c r="A28" s="35">
         <v>27</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="29">
+      <c r="D28" s="30"/>
+      <c r="E28" s="31">
         <v>2</v>
       </c>
-      <c r="F28" s="29">
+      <c r="F28" s="31">
         <v>37</v>
       </c>
-      <c r="G28" s="29">
+      <c r="G28" s="31">
         <v>8</v>
       </c>
-      <c r="H28" s="29">
-        <v>0</v>
-      </c>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29" t="s">
+      <c r="H28" s="31">
+        <v>0</v>
+      </c>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="29" t="s">
+      <c r="K28" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="L28" s="28" t="s">
+      <c r="L28" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="M28" s="28"/>
-      <c r="N28" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="O28" s="38" t="s">
+      <c r="M28" s="30"/>
+      <c r="N28" s="32" t="s">
         <v>272</v>
       </c>
+      <c r="O28" s="40" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="32">
+      <c r="A29" s="35">
         <v>28</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="29">
+      <c r="D29" s="30"/>
+      <c r="E29" s="31">
         <v>2</v>
       </c>
-      <c r="F29" s="29">
+      <c r="F29" s="31">
         <v>22</v>
       </c>
-      <c r="G29" s="29">
+      <c r="G29" s="31">
         <v>8</v>
       </c>
-      <c r="H29" s="29">
-        <v>0</v>
-      </c>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29" t="s">
+      <c r="H29" s="31">
+        <v>0</v>
+      </c>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="K29" s="29" t="s">
+      <c r="K29" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="L29" s="28" t="s">
+      <c r="L29" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="M29" s="28"/>
-      <c r="N29" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="O29" s="38" t="s">
+      <c r="M29" s="30"/>
+      <c r="N29" s="32" t="s">
         <v>272</v>
       </c>
+      <c r="O29" s="40" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="32">
+      <c r="A30" s="35">
         <v>29</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="29">
+      <c r="D30" s="30"/>
+      <c r="E30" s="31">
         <v>6</v>
       </c>
-      <c r="F30" s="29">
+      <c r="F30" s="31">
         <v>14</v>
       </c>
-      <c r="G30" s="29">
-        <v>16</v>
-      </c>
-      <c r="H30" s="29">
-        <v>0</v>
-      </c>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29" t="s">
+      <c r="G30" s="31">
+        <v>16</v>
+      </c>
+      <c r="H30" s="31">
+        <v>0</v>
+      </c>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="K30" s="29" t="s">
+      <c r="K30" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="O30" s="38" t="s">
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="32" t="s">
         <v>272</v>
       </c>
+      <c r="O30" s="40" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="32">
-        <v>30</v>
-      </c>
-      <c r="B31" s="28" t="s">
+      <c r="A31" s="35">
+        <v>30</v>
+      </c>
+      <c r="B31" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="29">
+      <c r="D31" s="30"/>
+      <c r="E31" s="31">
         <v>1</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="31">
         <v>4</v>
       </c>
-      <c r="G31" s="29">
+      <c r="G31" s="31">
         <v>56</v>
       </c>
-      <c r="H31" s="29">
-        <v>0</v>
-      </c>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29" t="s">
+      <c r="H31" s="31">
+        <v>0</v>
+      </c>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="K31" s="29" t="s">
+      <c r="K31" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="O31" s="38" t="s">
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="N31" s="32" t="s">
         <v>272</v>
+      </c>
+      <c r="O31" s="40" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -3029,11 +3048,11 @@
         <v>78</v>
       </c>
       <c r="M32" s="4"/>
-      <c r="N32" s="30" t="s">
+      <c r="N32" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O32" s="37" t="s">
-        <v>273</v>
+      <c r="O32" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
@@ -3072,11 +3091,11 @@
         <v>50</v>
       </c>
       <c r="M33" s="4"/>
-      <c r="N33" s="30" t="s">
+      <c r="N33" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O33" s="37" t="s">
-        <v>273</v>
+      <c r="O33" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -3115,11 +3134,11 @@
         <v>50</v>
       </c>
       <c r="M34" s="4"/>
-      <c r="N34" s="30" t="s">
+      <c r="N34" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O34" s="37" t="s">
-        <v>273</v>
+      <c r="O34" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -3158,11 +3177,11 @@
         <v>50</v>
       </c>
       <c r="M35" s="4"/>
-      <c r="N35" s="30" t="s">
+      <c r="N35" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O35" s="37" t="s">
-        <v>273</v>
+      <c r="O35" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -3201,11 +3220,11 @@
         <v>50</v>
       </c>
       <c r="M36" s="4"/>
-      <c r="N36" s="30" t="s">
+      <c r="N36" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O36" s="37" t="s">
-        <v>273</v>
+      <c r="O36" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
@@ -3244,11 +3263,11 @@
         <v>75</v>
       </c>
       <c r="M37" s="6"/>
-      <c r="N37" s="30" t="s">
+      <c r="N37" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O37" s="37" t="s">
-        <v>273</v>
+      <c r="O37" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -3287,11 +3306,11 @@
         <v>50</v>
       </c>
       <c r="M38" s="4"/>
-      <c r="N38" s="30" t="s">
+      <c r="N38" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O38" s="37" t="s">
-        <v>273</v>
+      <c r="O38" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
@@ -3330,11 +3349,11 @@
         <v>50</v>
       </c>
       <c r="M39" s="4"/>
-      <c r="N39" s="30" t="s">
+      <c r="N39" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O39" s="37" t="s">
-        <v>273</v>
+      <c r="O39" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -3373,11 +3392,11 @@
         <v>50</v>
       </c>
       <c r="M40" s="9"/>
-      <c r="N40" s="30" t="s">
+      <c r="N40" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O40" s="37" t="s">
-        <v>273</v>
+      <c r="O40" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -3416,11 +3435,11 @@
         <v>50</v>
       </c>
       <c r="M41" s="4"/>
-      <c r="N41" s="30" t="s">
+      <c r="N41" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O41" s="37" t="s">
-        <v>273</v>
+      <c r="O41" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -3459,11 +3478,11 @@
         <v>107</v>
       </c>
       <c r="M42" s="4"/>
-      <c r="N42" s="30" t="s">
+      <c r="N42" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O42" s="37" t="s">
-        <v>273</v>
+      <c r="O42" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -3502,11 +3521,11 @@
         <v>50</v>
       </c>
       <c r="M43" s="4"/>
-      <c r="N43" s="30" t="s">
+      <c r="N43" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O43" s="37" t="s">
-        <v>273</v>
+      <c r="O43" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -3545,11 +3564,11 @@
         <v>50</v>
       </c>
       <c r="M44" s="6"/>
-      <c r="N44" s="30" t="s">
+      <c r="N44" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O44" s="37" t="s">
-        <v>273</v>
+      <c r="O44" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -3588,11 +3607,11 @@
         <v>50</v>
       </c>
       <c r="M45" s="6"/>
-      <c r="N45" s="30" t="s">
+      <c r="N45" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O45" s="37" t="s">
-        <v>273</v>
+      <c r="O45" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
@@ -3633,11 +3652,11 @@
         <v>50</v>
       </c>
       <c r="M46" s="6"/>
-      <c r="N46" s="30" t="s">
+      <c r="N46" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O46" s="37" t="s">
-        <v>273</v>
+      <c r="O46" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
@@ -3678,11 +3697,11 @@
         <v>50</v>
       </c>
       <c r="M47" s="6"/>
-      <c r="N47" s="30" t="s">
+      <c r="N47" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="O47" s="37" t="s">
-        <v>273</v>
+      <c r="O47" s="40" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
@@ -3721,14 +3740,14 @@
         <v>50</v>
       </c>
       <c r="M48" s="4"/>
-      <c r="N48" s="30" t="s">
+      <c r="N48" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="O48" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O48" s="40" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3763,15 +3782,15 @@
       <c r="L49" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="M49" s="24"/>
-      <c r="N49" s="30" t="s">
+      <c r="M49" s="26"/>
+      <c r="N49" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="O49" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O49" s="40" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3806,15 +3825,15 @@
       <c r="L50" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="M50" s="24"/>
-      <c r="N50" s="30" t="s">
+      <c r="M50" s="26"/>
+      <c r="N50" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="O50" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O50" s="40" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3849,15 +3868,15 @@
       <c r="L51" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="M51" s="24"/>
-      <c r="N51" s="30" t="s">
+      <c r="M51" s="26"/>
+      <c r="N51" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="O51" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O51" s="40" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3893,14 +3912,14 @@
         <v>122</v>
       </c>
       <c r="M52" s="4"/>
-      <c r="N52" s="30" t="s">
+      <c r="N52" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="O52" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O52" s="40" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3935,15 +3954,15 @@
       <c r="L53" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="M53" s="24"/>
-      <c r="N53" s="30" t="s">
+      <c r="M53" s="26"/>
+      <c r="N53" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="O53" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O53" s="40" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3979,14 +3998,14 @@
         <v>72</v>
       </c>
       <c r="M54" s="4"/>
-      <c r="N54" s="30" t="s">
+      <c r="N54" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="O54" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O54" s="40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4022,14 +4041,14 @@
         <v>50</v>
       </c>
       <c r="M55" s="4"/>
-      <c r="N55" s="30" t="s">
+      <c r="N55" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="O55" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O55" s="40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4065,14 +4084,14 @@
         <v>165</v>
       </c>
       <c r="M56" s="4"/>
-      <c r="N56" s="30" t="s">
+      <c r="N56" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="O56" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O56" s="40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4108,14 +4127,14 @@
         <v>171</v>
       </c>
       <c r="M57" s="4"/>
-      <c r="N57" s="30" t="s">
+      <c r="N57" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="O57" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O57" s="40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4151,14 +4170,14 @@
         <v>50</v>
       </c>
       <c r="M58" s="4"/>
-      <c r="N58" s="30" t="s">
+      <c r="N58" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="O58" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O58" s="40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4194,14 +4213,14 @@
         <v>50</v>
       </c>
       <c r="M59" s="4"/>
-      <c r="N59" s="30" t="s">
+      <c r="N59" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="O59" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O59" s="40" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16">
         <v>59</v>
       </c>
@@ -4237,18 +4256,17 @@
         <v>110</v>
       </c>
       <c r="M60" s="18"/>
-      <c r="N60" s="30" t="s">
+      <c r="N60" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="O60" s="37" t="s">
-        <v>276</v>
+      <c r="O60" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="P60" s="14"/>
       <c r="Q60" s="14"/>
       <c r="R60" s="14"/>
-      <c r="S60" s="14"/>
-    </row>
-    <row r="61" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16">
         <v>60</v>
       </c>
@@ -4284,18 +4302,17 @@
         <v>110</v>
       </c>
       <c r="M61" s="18"/>
-      <c r="N61" s="30" t="s">
+      <c r="N61" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="O61" s="37" t="s">
-        <v>276</v>
+      <c r="O61" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="P61" s="14"/>
       <c r="Q61" s="14"/>
       <c r="R61" s="14"/>
-      <c r="S61" s="14"/>
-    </row>
-    <row r="62" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16">
         <v>61</v>
       </c>
@@ -4331,18 +4348,17 @@
         <v>110</v>
       </c>
       <c r="M62" s="18"/>
-      <c r="N62" s="30" t="s">
+      <c r="N62" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="O62" s="37" t="s">
-        <v>276</v>
+      <c r="O62" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="P62" s="14"/>
       <c r="Q62" s="14"/>
       <c r="R62" s="14"/>
-      <c r="S62" s="14"/>
-    </row>
-    <row r="63" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16">
         <v>62</v>
       </c>
@@ -4378,18 +4394,17 @@
         <v>122</v>
       </c>
       <c r="M63" s="18"/>
-      <c r="N63" s="30" t="s">
+      <c r="N63" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="O63" s="37" t="s">
-        <v>276</v>
+      <c r="O63" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="P63" s="14"/>
       <c r="Q63" s="14"/>
       <c r="R63" s="14"/>
-      <c r="S63" s="14"/>
-    </row>
-    <row r="64" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16">
         <v>63</v>
       </c>
@@ -4425,18 +4440,17 @@
         <v>78</v>
       </c>
       <c r="M64" s="18"/>
-      <c r="N64" s="30" t="s">
+      <c r="N64" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="O64" s="37" t="s">
-        <v>276</v>
+      <c r="O64" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="P64" s="14"/>
       <c r="Q64" s="14"/>
       <c r="R64" s="14"/>
-      <c r="S64" s="14"/>
-    </row>
-    <row r="65" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16">
         <v>64</v>
       </c>
@@ -4472,18 +4486,17 @@
         <v>107</v>
       </c>
       <c r="M65" s="18"/>
-      <c r="N65" s="30" t="s">
+      <c r="N65" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="O65" s="37" t="s">
-        <v>276</v>
+      <c r="O65" s="40" t="s">
+        <v>278</v>
       </c>
       <c r="P65" s="14"/>
       <c r="Q65" s="14"/>
       <c r="R65" s="14"/>
-      <c r="S65" s="14"/>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4519,14 +4532,14 @@
         <v>134</v>
       </c>
       <c r="M66" s="4"/>
-      <c r="N66" s="30" t="s">
+      <c r="N66" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O66" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O66" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4561,15 +4574,15 @@
       <c r="L67" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M67" s="24"/>
-      <c r="N67" s="30" t="s">
+      <c r="M67" s="26"/>
+      <c r="N67" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O67" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O67" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4605,14 +4618,14 @@
         <v>50</v>
       </c>
       <c r="M68" s="4"/>
-      <c r="N68" s="30" t="s">
+      <c r="N68" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O68" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O68" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -4648,14 +4661,14 @@
         <v>155</v>
       </c>
       <c r="M69" s="4"/>
-      <c r="N69" s="30" t="s">
+      <c r="N69" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O69" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O69" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -4691,64 +4704,68 @@
         <v>217</v>
       </c>
       <c r="M70" s="4"/>
-      <c r="N70" s="30" t="s">
+      <c r="N70" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O70" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O70" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
-        <v>72</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D71" s="6"/>
-      <c r="E71" s="7">
-        <v>3</v>
-      </c>
-      <c r="F71" s="7">
-        <v>30</v>
-      </c>
-      <c r="G71" s="7">
-        <v>30</v>
-      </c>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E71" s="5">
+        <v>3</v>
+      </c>
+      <c r="F71" s="5">
+        <v>30</v>
+      </c>
+      <c r="G71" s="5">
+        <v>30</v>
+      </c>
+      <c r="H71" s="5">
+        <v>0</v>
+      </c>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K71" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L71" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="M71" s="6"/>
-      <c r="N71" s="30" t="s">
+      <c r="K71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M71" s="4"/>
+      <c r="N71" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O71" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O71" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E72" s="5">
         <v>3</v>
@@ -4773,68 +4790,64 @@
         <v>50</v>
       </c>
       <c r="M72" s="4"/>
-      <c r="N72" s="30" t="s">
+      <c r="N72" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O72" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O72" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
-        <v>74</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="E73" s="5">
-        <v>3</v>
-      </c>
-      <c r="F73" s="5">
-        <v>0</v>
-      </c>
-      <c r="G73" s="5">
-        <v>0</v>
-      </c>
-      <c r="H73" s="5">
-        <v>0</v>
-      </c>
-      <c r="I73" s="5"/>
-      <c r="J73" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="D73" s="6"/>
+      <c r="E73" s="7">
+        <v>3</v>
+      </c>
+      <c r="F73" s="7">
+        <v>30</v>
+      </c>
+      <c r="G73" s="7">
+        <v>30</v>
+      </c>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+      <c r="J73" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K73" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L73" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M73" s="4"/>
-      <c r="N73" s="30" t="s">
+      <c r="K73" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L73" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="M73" s="6"/>
+      <c r="N73" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O73" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O73" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="E74" s="5">
         <v>3</v>
@@ -4859,25 +4872,25 @@
         <v>50</v>
       </c>
       <c r="M74" s="4"/>
-      <c r="N74" s="30" t="s">
+      <c r="N74" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O74" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O74" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="E75" s="5">
         <v>3</v>
@@ -4902,34 +4915,34 @@
         <v>50</v>
       </c>
       <c r="M75" s="4"/>
-      <c r="N75" s="30" t="s">
+      <c r="N75" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O75" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O75" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="E76" s="5">
         <v>3</v>
       </c>
       <c r="F76" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G76" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H76" s="5">
         <v>0</v>
@@ -4945,81 +4958,77 @@
         <v>50</v>
       </c>
       <c r="M76" s="4"/>
-      <c r="N76" s="30" t="s">
+      <c r="N76" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O76" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="77" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O76" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <v>78</v>
-      </c>
-      <c r="B77" s="19" t="s">
-        <v>235</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>236</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="E77" s="13">
-        <v>3</v>
-      </c>
-      <c r="F77" s="13">
-        <v>30</v>
-      </c>
-      <c r="G77" s="13">
-        <v>30</v>
-      </c>
-      <c r="H77" s="13">
-        <v>0</v>
-      </c>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E77" s="5">
+        <v>3</v>
+      </c>
+      <c r="F77" s="5">
+        <v>0</v>
+      </c>
+      <c r="G77" s="5">
+        <v>0</v>
+      </c>
+      <c r="H77" s="5">
+        <v>0</v>
+      </c>
+      <c r="I77" s="5"/>
+      <c r="J77" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K77" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L77" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="M77" s="18"/>
-      <c r="N77" s="30" t="s">
+      <c r="K77" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L77" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M77" s="4"/>
+      <c r="N77" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O77" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="P77" s="14"/>
-      <c r="Q77" s="14"/>
-      <c r="R77" s="14"/>
-      <c r="S77" s="14"/>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="O77" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
-        <v>79</v>
-      </c>
-      <c r="B78" s="19" t="s">
-        <v>238</v>
+        <v>77</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>221</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
       <c r="E78" s="5">
         <v>3</v>
       </c>
       <c r="F78" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="G78" s="5">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="H78" s="5">
         <v>0</v>
@@ -5029,121 +5038,120 @@
         <v>4</v>
       </c>
       <c r="K78" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L78" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M78" s="4"/>
+      <c r="N78" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="O78" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>78</v>
+      </c>
+      <c r="B79" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="D79" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="E79" s="13">
+        <v>3</v>
+      </c>
+      <c r="F79" s="13">
+        <v>30</v>
+      </c>
+      <c r="G79" s="13">
+        <v>30</v>
+      </c>
+      <c r="H79" s="13">
+        <v>0</v>
+      </c>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K79" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="L79" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="M79" s="18"/>
+      <c r="N79" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="O79" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="P79" s="14"/>
+      <c r="Q79" s="14"/>
+      <c r="R79" s="14"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A80" s="3">
+        <v>79</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E80" s="5">
+        <v>3</v>
+      </c>
+      <c r="F80" s="5">
+        <v>30</v>
+      </c>
+      <c r="G80" s="5">
+        <v>30</v>
+      </c>
+      <c r="H80" s="5">
+        <v>0</v>
+      </c>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K80" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="L78" s="4" t="s">
+      <c r="L80" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="M78" s="18"/>
-      <c r="N78" s="30" t="s">
+      <c r="M80" s="18"/>
+      <c r="N80" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O78" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A79" s="3">
+      <c r="O80" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A81" s="3">
         <v>80</v>
       </c>
-      <c r="B79" s="19" t="s">
+      <c r="B81" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="C79" s="4" t="s">
+      <c r="C81" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="D79" s="4" t="s">
+      <c r="D81" s="4" t="s">
         <v>243</v>
-      </c>
-      <c r="E79" s="5">
-        <v>3</v>
-      </c>
-      <c r="F79" s="5">
-        <v>30</v>
-      </c>
-      <c r="G79" s="5">
-        <v>30</v>
-      </c>
-      <c r="H79" s="5">
-        <v>0</v>
-      </c>
-      <c r="I79" s="5"/>
-      <c r="J79" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="K79" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="L79" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M79" s="18"/>
-      <c r="N79" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="O79" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="80" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3">
-        <v>81</v>
-      </c>
-      <c r="B80" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="D80" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="E80" s="13">
-        <v>3</v>
-      </c>
-      <c r="F80" s="13">
-        <v>30</v>
-      </c>
-      <c r="G80" s="13">
-        <v>30</v>
-      </c>
-      <c r="H80" s="13">
-        <v>0</v>
-      </c>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="K80" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="L80" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M80" s="18"/>
-      <c r="N80" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="O80" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="P80" s="14"/>
-      <c r="Q80" s="14"/>
-      <c r="R80" s="14"/>
-      <c r="S80" s="14"/>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A81" s="3">
-        <v>82</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="C81" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>249</v>
       </c>
       <c r="E81" s="5">
         <v>3</v>
@@ -5162,225 +5170,315 @@
         <v>4</v>
       </c>
       <c r="K81" s="5" t="s">
-        <v>189</v>
+        <v>68</v>
       </c>
       <c r="L81" s="4" t="s">
         <v>110</v>
       </c>
       <c r="M81" s="18"/>
-      <c r="N81" s="30" t="s">
+      <c r="N81" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="O81" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="O81" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="82" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>83</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="E82" s="5">
-        <v>2</v>
-      </c>
-      <c r="F82" s="5">
-        <v>0</v>
-      </c>
-      <c r="G82" s="5">
-        <v>0</v>
-      </c>
-      <c r="H82" s="5">
-        <v>60</v>
-      </c>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="K82" s="5" t="s">
-        <v>253</v>
+        <v>81</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="E82" s="13">
+        <v>3</v>
+      </c>
+      <c r="F82" s="13">
+        <v>30</v>
+      </c>
+      <c r="G82" s="13">
+        <v>30</v>
+      </c>
+      <c r="H82" s="13">
+        <v>0</v>
+      </c>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="K82" s="13" t="s">
+        <v>68</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M82" s="4"/>
-      <c r="N82" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="O82" s="38" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+      <c r="M82" s="18"/>
+      <c r="N82" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="O82" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="P82" s="14"/>
+      <c r="Q82" s="14"/>
+      <c r="R82" s="14"/>
+    </row>
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
-        <v>84</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>254</v>
+        <v>82</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>247</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="E83" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F83" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="G83" s="5">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H83" s="5">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="I83" s="5"/>
       <c r="J83" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K83" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="L83" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M83" s="18"/>
+      <c r="N83" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="O83" s="40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="3">
+        <v>83</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E84" s="5">
+        <v>2</v>
+      </c>
+      <c r="F84" s="5">
+        <v>0</v>
+      </c>
+      <c r="G84" s="5">
+        <v>0</v>
+      </c>
+      <c r="H84" s="5">
+        <v>60</v>
+      </c>
+      <c r="I84" s="5"/>
+      <c r="J84" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K83" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="L83" s="4" t="s">
+      <c r="K84" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="L84" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M84" s="4"/>
+      <c r="N84" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="O84" s="41" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A85" s="3">
+        <v>84</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E85" s="5">
+        <v>2</v>
+      </c>
+      <c r="F85" s="5">
+        <v>0</v>
+      </c>
+      <c r="G85" s="5">
+        <v>0</v>
+      </c>
+      <c r="H85" s="5">
+        <v>60</v>
+      </c>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K85" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L85" s="43" t="s">
         <v>257</v>
       </c>
-      <c r="M83" s="4"/>
-      <c r="N83" s="30" t="s">
+      <c r="M85" s="4"/>
+      <c r="N85" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="O83" s="38" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="20">
+      <c r="O85" s="41" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="86" spans="1:18" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="20">
         <v>85</v>
       </c>
-      <c r="B84" s="40" t="s">
+      <c r="B86" s="23" t="s">
         <v>258</v>
       </c>
-      <c r="C84" s="40" t="s">
+      <c r="C86" s="23" t="s">
         <v>259</v>
       </c>
-      <c r="D84" s="40" t="s">
+      <c r="D86" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="E84" s="41">
+      <c r="E86" s="24">
         <v>6</v>
       </c>
-      <c r="F84" s="41">
-        <v>0</v>
-      </c>
-      <c r="G84" s="41">
-        <v>0</v>
-      </c>
-      <c r="H84" s="41"/>
-      <c r="I84" s="41">
+      <c r="F86" s="24">
+        <v>0</v>
+      </c>
+      <c r="G86" s="24">
+        <v>0</v>
+      </c>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24">
         <v>180</v>
       </c>
-      <c r="J84" s="41" t="s">
+      <c r="J86" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="K84" s="42" t="s">
+      <c r="K86" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="L84" s="40" t="s">
+      <c r="L86" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="M84" s="40"/>
-      <c r="N84" s="31" t="s">
+      <c r="M86" s="23"/>
+      <c r="N86" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="O84" s="39" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A85" s="21"/>
-      <c r="B85" s="22"/>
-      <c r="C85" s="22"/>
-      <c r="D85" s="22"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="21"/>
-      <c r="G85" s="21"/>
-      <c r="H85" s="21"/>
-      <c r="I85" s="21"/>
-      <c r="J85" s="21"/>
-      <c r="K85" s="21"/>
-      <c r="L85" s="22"/>
-      <c r="M85" s="22"/>
+      <c r="O86" s="42" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A87" s="21"/>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="21"/>
+      <c r="H87" s="21"/>
+      <c r="I87" s="21"/>
+      <c r="J87" s="21"/>
+      <c r="K87" s="21"/>
+      <c r="L87" s="22"/>
+      <c r="M87" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L50">
+    <cfRule type="expression" dxfId="9" priority="5">
+      <formula>#REF!=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L53">
     <cfRule type="expression" dxfId="8" priority="4">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L53">
+  <conditionalFormatting sqref="J46:J47">
     <cfRule type="expression" dxfId="7" priority="3">
+      <formula>$K46&lt;&gt;#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K46:M47 B73:K73 M73 B74:M86 B48:M72 B2:M45 N2:N86">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J46:J47">
-    <cfRule type="expression" dxfId="6" priority="2">
-      <formula>$K46&lt;&gt;#REF!</formula>
+  <conditionalFormatting sqref="B48:C86 B2:C45">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:M47 B71:K71 M71 B72:M84 B48:M70 B2:M45 N2:O84">
-    <cfRule type="expression" dxfId="5" priority="5">
+  <conditionalFormatting sqref="L70 L67 B61:B65 B79:B83">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:C45 B48:C84">
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>#REF!=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L70 L67 B61:B65 B77:B81">
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>#REF!=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L50 L71 L53">
-    <cfRule type="expression" dxfId="2" priority="8">
+  <conditionalFormatting sqref="L50 L73 L53">
+    <cfRule type="expression" dxfId="3" priority="9">
       <formula>#REF!&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:J47">
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" dxfId="2" priority="10">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:C47">
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O86">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>#REF!=1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="07db5020-ba8e-48bf-aa17-fbace2a70736">
-      <UserInfo>
-        <DisplayName>CAP K24T-TEAM01 Members</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5532,20 +5630,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="07db5020-ba8e-48bf-aa17-fbace2a70736">
+      <UserInfo>
+        <DisplayName>CAP K24T-TEAM01 Members</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{179DDC9E-E391-4AD2-A488-D9C201286EF9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5569,9 +5670,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{179DDC9E-E391-4AD2-A488-D9C201286EF9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Import study program
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BA1C99-3508-40C1-B595-AC7E683E2807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E32EAC7-7E6D-4662-A02B-402B3FBBBF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -1106,7 +1106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1142,9 +1142,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1162,10 +1159,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1707,11 +1700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE44191-4F7D-454A-9855-FE690642DDD6}">
-  <dimension ref="A1:R87"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L87" sqref="L87"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1728,53 +1721,52 @@
     <col min="13" max="13" width="24.21875" customWidth="1"/>
     <col min="14" max="14" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="33.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="36" t="s">
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="36" t="s">
+      <c r="D1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="33" t="s">
         <v>268</v>
       </c>
-      <c r="K1" s="38" t="s">
+      <c r="K1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="L1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="N1" s="33" t="s">
         <v>270</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="36" t="s">
         <v>269</v>
       </c>
     </row>
@@ -1812,10 +1804,10 @@
         <v>16</v>
       </c>
       <c r="M2" s="4"/>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -1853,10 +1845,10 @@
         <v>12</v>
       </c>
       <c r="M3" s="4"/>
-      <c r="N3" s="32" t="s">
+      <c r="N3" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="O3" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -1894,10 +1886,10 @@
         <v>12</v>
       </c>
       <c r="M4" s="4"/>
-      <c r="N4" s="32" t="s">
+      <c r="N4" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="O4" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -1935,10 +1927,10 @@
         <v>17</v>
       </c>
       <c r="M5" s="4"/>
-      <c r="N5" s="32" t="s">
+      <c r="N5" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -1976,24 +1968,24 @@
         <v>25</v>
       </c>
       <c r="M6" s="4"/>
-      <c r="N6" s="32" t="s">
+      <c r="N6" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="O6" s="37" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="A7" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="13">
         <v>3</v>
       </c>
@@ -2013,14 +2005,14 @@
       <c r="K7" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="25" t="s">
+      <c r="L7" s="17"/>
+      <c r="M7" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="N7" s="32" t="s">
+      <c r="N7" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O7" s="40" t="s">
+      <c r="O7" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2056,10 +2048,10 @@
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="32" t="s">
+      <c r="N8" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O8" s="40" t="s">
+      <c r="O8" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2095,10 +2087,10 @@
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="32" t="s">
+      <c r="N9" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O9" s="40" t="s">
+      <c r="O9" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2134,10 +2126,10 @@
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
-      <c r="N10" s="32" t="s">
+      <c r="N10" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O10" s="40" t="s">
+      <c r="O10" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2173,10 +2165,10 @@
       </c>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
-      <c r="N11" s="32" t="s">
+      <c r="N11" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O11" s="40" t="s">
+      <c r="O11" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2212,10 +2204,10 @@
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
-      <c r="N12" s="32" t="s">
+      <c r="N12" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O12" s="40" t="s">
+      <c r="O12" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2251,10 +2243,10 @@
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
-      <c r="N13" s="32" t="s">
+      <c r="N13" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O13" s="40" t="s">
+      <c r="O13" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2292,10 +2284,10 @@
         <v>50</v>
       </c>
       <c r="M14" s="4"/>
-      <c r="N14" s="32" t="s">
+      <c r="N14" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O14" s="40" t="s">
+      <c r="O14" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2333,10 +2325,10 @@
         <v>50</v>
       </c>
       <c r="M15" s="4"/>
-      <c r="N15" s="32" t="s">
+      <c r="N15" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O15" s="40" t="s">
+      <c r="O15" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2376,10 +2368,10 @@
         <v>50</v>
       </c>
       <c r="M16" s="4"/>
-      <c r="N16" s="32" t="s">
+      <c r="N16" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O16" s="40" t="s">
+      <c r="O16" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2419,10 +2411,10 @@
         <v>50</v>
       </c>
       <c r="M17" s="6"/>
-      <c r="N17" s="32" t="s">
+      <c r="N17" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O17" s="40" t="s">
+      <c r="O17" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2462,10 +2454,10 @@
         <v>50</v>
       </c>
       <c r="M18" s="4"/>
-      <c r="N18" s="32" t="s">
+      <c r="N18" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O18" s="40" t="s">
+      <c r="O18" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2505,10 +2497,10 @@
         <v>15</v>
       </c>
       <c r="M19" s="6"/>
-      <c r="N19" s="32" t="s">
+      <c r="N19" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O19" s="40" t="s">
+      <c r="O19" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2548,10 +2540,10 @@
         <v>68</v>
       </c>
       <c r="M20" s="4"/>
-      <c r="N20" s="32" t="s">
+      <c r="N20" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O20" s="40" t="s">
+      <c r="O20" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2591,10 +2583,10 @@
         <v>68</v>
       </c>
       <c r="M21" s="4"/>
-      <c r="N21" s="32" t="s">
+      <c r="N21" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O21" s="40" t="s">
+      <c r="O21" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2634,10 +2626,10 @@
         <v>50</v>
       </c>
       <c r="M22" s="4"/>
-      <c r="N22" s="32" t="s">
+      <c r="N22" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O22" s="40" t="s">
+      <c r="O22" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2677,10 +2669,10 @@
         <v>50</v>
       </c>
       <c r="M23" s="4"/>
-      <c r="N23" s="32" t="s">
+      <c r="N23" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O23" s="40" t="s">
+      <c r="O23" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2720,10 +2712,10 @@
         <v>50</v>
       </c>
       <c r="M24" s="4"/>
-      <c r="N24" s="32" t="s">
+      <c r="N24" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O24" s="40" t="s">
+      <c r="O24" s="37" t="s">
         <v>271</v>
       </c>
     </row>
@@ -2763,252 +2755,252 @@
         <v>50</v>
       </c>
       <c r="M25" s="4"/>
-      <c r="N25" s="32" t="s">
+      <c r="N25" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O25" s="40" t="s">
+      <c r="O25" s="37" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="35">
+      <c r="A26" s="32">
         <v>25</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="28">
+      <c r="D26" s="24"/>
+      <c r="E26" s="25">
         <v>2</v>
       </c>
-      <c r="F26" s="29">
-        <v>0</v>
-      </c>
-      <c r="G26" s="29">
+      <c r="F26" s="26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="26">
         <v>60</v>
       </c>
-      <c r="H26" s="29">
-        <v>0</v>
-      </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29" t="s">
+      <c r="H26" s="26">
+        <v>0</v>
+      </c>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K26" s="29" t="s">
+      <c r="K26" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="L26" s="27" t="s">
+      <c r="L26" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="M26" s="27"/>
-      <c r="N26" s="32" t="s">
+      <c r="M26" s="24"/>
+      <c r="N26" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="O26" s="40" t="s">
+      <c r="O26" s="37" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="35">
+      <c r="A27" s="32">
         <v>26</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28">
+      <c r="D27" s="24"/>
+      <c r="E27" s="25">
         <v>2</v>
       </c>
-      <c r="F27" s="29">
-        <v>0</v>
-      </c>
-      <c r="G27" s="29">
+      <c r="F27" s="26">
+        <v>0</v>
+      </c>
+      <c r="G27" s="26">
         <v>60</v>
       </c>
-      <c r="H27" s="29">
-        <v>0</v>
-      </c>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29" t="s">
+      <c r="H27" s="26">
+        <v>0</v>
+      </c>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="K27" s="29" t="s">
+      <c r="K27" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="L27" s="27" t="s">
+      <c r="L27" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="M27" s="27"/>
-      <c r="N27" s="32" t="s">
+      <c r="M27" s="24"/>
+      <c r="N27" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="O27" s="40" t="s">
+      <c r="O27" s="37" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="35">
+      <c r="A28" s="32">
         <v>27</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31">
+      <c r="D28" s="27"/>
+      <c r="E28" s="28">
         <v>2</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="28">
         <v>37</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="28">
         <v>8</v>
       </c>
-      <c r="H28" s="31">
-        <v>0</v>
-      </c>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31" t="s">
+      <c r="H28" s="28">
+        <v>0</v>
+      </c>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="31" t="s">
+      <c r="K28" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="L28" s="30" t="s">
+      <c r="L28" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="M28" s="30"/>
-      <c r="N28" s="32" t="s">
+      <c r="M28" s="27"/>
+      <c r="N28" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="O28" s="40" t="s">
+      <c r="O28" s="37" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="35">
+      <c r="A29" s="32">
         <v>28</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31">
+      <c r="D29" s="27"/>
+      <c r="E29" s="28">
         <v>2</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="28">
         <v>22</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="28">
         <v>8</v>
       </c>
-      <c r="H29" s="31">
-        <v>0</v>
-      </c>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31" t="s">
+      <c r="H29" s="28">
+        <v>0</v>
+      </c>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="K29" s="31" t="s">
+      <c r="K29" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="L29" s="30" t="s">
+      <c r="L29" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="M29" s="30"/>
-      <c r="N29" s="32" t="s">
+      <c r="M29" s="27"/>
+      <c r="N29" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="O29" s="40" t="s">
+      <c r="O29" s="37" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="35">
+      <c r="A30" s="32">
         <v>29</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31">
+      <c r="D30" s="27"/>
+      <c r="E30" s="28">
         <v>6</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="28">
         <v>14</v>
       </c>
-      <c r="G30" s="31">
-        <v>16</v>
-      </c>
-      <c r="H30" s="31">
-        <v>0</v>
-      </c>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31" t="s">
+      <c r="G30" s="28">
+        <v>16</v>
+      </c>
+      <c r="H30" s="28">
+        <v>0</v>
+      </c>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="K30" s="31" t="s">
+      <c r="K30" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L30" s="30"/>
-      <c r="M30" s="30"/>
-      <c r="N30" s="32" t="s">
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+      <c r="N30" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="O30" s="40" t="s">
+      <c r="O30" s="37" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="35">
-        <v>30</v>
-      </c>
-      <c r="B31" s="30" t="s">
+      <c r="A31" s="32">
+        <v>30</v>
+      </c>
+      <c r="B31" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="31">
+      <c r="D31" s="27"/>
+      <c r="E31" s="28">
         <v>1</v>
       </c>
-      <c r="F31" s="31">
+      <c r="F31" s="28">
         <v>4</v>
       </c>
-      <c r="G31" s="31">
+      <c r="G31" s="28">
         <v>56</v>
       </c>
-      <c r="H31" s="31">
-        <v>0</v>
-      </c>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31" t="s">
+      <c r="H31" s="28">
+        <v>0</v>
+      </c>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="K31" s="31" t="s">
+      <c r="K31" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="32" t="s">
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
+      <c r="N31" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="O31" s="40" t="s">
+      <c r="O31" s="37" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3048,10 +3040,10 @@
         <v>78</v>
       </c>
       <c r="M32" s="4"/>
-      <c r="N32" s="32" t="s">
+      <c r="N32" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O32" s="40" t="s">
+      <c r="O32" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3091,10 +3083,10 @@
         <v>50</v>
       </c>
       <c r="M33" s="4"/>
-      <c r="N33" s="32" t="s">
+      <c r="N33" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O33" s="40" t="s">
+      <c r="O33" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3134,10 +3126,10 @@
         <v>50</v>
       </c>
       <c r="M34" s="4"/>
-      <c r="N34" s="32" t="s">
+      <c r="N34" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O34" s="40" t="s">
+      <c r="O34" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3177,10 +3169,10 @@
         <v>50</v>
       </c>
       <c r="M35" s="4"/>
-      <c r="N35" s="32" t="s">
+      <c r="N35" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O35" s="40" t="s">
+      <c r="O35" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3220,10 +3212,10 @@
         <v>50</v>
       </c>
       <c r="M36" s="4"/>
-      <c r="N36" s="32" t="s">
+      <c r="N36" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O36" s="40" t="s">
+      <c r="O36" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3263,10 +3255,10 @@
         <v>75</v>
       </c>
       <c r="M37" s="6"/>
-      <c r="N37" s="32" t="s">
+      <c r="N37" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O37" s="40" t="s">
+      <c r="O37" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3306,10 +3298,10 @@
         <v>50</v>
       </c>
       <c r="M38" s="4"/>
-      <c r="N38" s="32" t="s">
+      <c r="N38" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O38" s="40" t="s">
+      <c r="O38" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3349,10 +3341,10 @@
         <v>50</v>
       </c>
       <c r="M39" s="4"/>
-      <c r="N39" s="32" t="s">
+      <c r="N39" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O39" s="40" t="s">
+      <c r="O39" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3392,10 +3384,10 @@
         <v>50</v>
       </c>
       <c r="M40" s="9"/>
-      <c r="N40" s="32" t="s">
+      <c r="N40" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O40" s="40" t="s">
+      <c r="O40" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3435,10 +3427,10 @@
         <v>50</v>
       </c>
       <c r="M41" s="4"/>
-      <c r="N41" s="32" t="s">
+      <c r="N41" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O41" s="40" t="s">
+      <c r="O41" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3478,10 +3470,10 @@
         <v>107</v>
       </c>
       <c r="M42" s="4"/>
-      <c r="N42" s="32" t="s">
+      <c r="N42" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O42" s="40" t="s">
+      <c r="O42" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3521,10 +3513,10 @@
         <v>50</v>
       </c>
       <c r="M43" s="4"/>
-      <c r="N43" s="32" t="s">
+      <c r="N43" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O43" s="40" t="s">
+      <c r="O43" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3564,10 +3556,10 @@
         <v>50</v>
       </c>
       <c r="M44" s="6"/>
-      <c r="N44" s="32" t="s">
+      <c r="N44" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O44" s="40" t="s">
+      <c r="O44" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3607,10 +3599,10 @@
         <v>50</v>
       </c>
       <c r="M45" s="6"/>
-      <c r="N45" s="32" t="s">
+      <c r="N45" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O45" s="40" t="s">
+      <c r="O45" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3652,10 +3644,10 @@
         <v>50</v>
       </c>
       <c r="M46" s="6"/>
-      <c r="N46" s="32" t="s">
+      <c r="N46" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O46" s="40" t="s">
+      <c r="O46" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3697,10 +3689,10 @@
         <v>50</v>
       </c>
       <c r="M47" s="6"/>
-      <c r="N47" s="32" t="s">
+      <c r="N47" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O47" s="40" t="s">
+      <c r="O47" s="37" t="s">
         <v>274</v>
       </c>
     </row>
@@ -3740,14 +3732,14 @@
         <v>50</v>
       </c>
       <c r="M48" s="4"/>
-      <c r="N48" s="32" t="s">
+      <c r="N48" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O48" s="40" t="s">
+      <c r="O48" s="37" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3782,15 +3774,15 @@
       <c r="L49" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="M49" s="26"/>
-      <c r="N49" s="32" t="s">
+      <c r="M49" s="23"/>
+      <c r="N49" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O49" s="40" t="s">
+      <c r="O49" s="37" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3825,15 +3817,15 @@
       <c r="L50" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="M50" s="26"/>
-      <c r="N50" s="32" t="s">
+      <c r="M50" s="23"/>
+      <c r="N50" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O50" s="40" t="s">
+      <c r="O50" s="37" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3868,15 +3860,15 @@
       <c r="L51" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="M51" s="26"/>
-      <c r="N51" s="32" t="s">
+      <c r="M51" s="23"/>
+      <c r="N51" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O51" s="40" t="s">
+      <c r="O51" s="37" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3912,14 +3904,14 @@
         <v>122</v>
       </c>
       <c r="M52" s="4"/>
-      <c r="N52" s="32" t="s">
+      <c r="N52" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O52" s="40" t="s">
+      <c r="O52" s="37" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3954,15 +3946,15 @@
       <c r="L53" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="M53" s="26"/>
-      <c r="N53" s="32" t="s">
+      <c r="M53" s="23"/>
+      <c r="N53" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O53" s="40" t="s">
+      <c r="O53" s="37" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -3998,14 +3990,14 @@
         <v>72</v>
       </c>
       <c r="M54" s="4"/>
-      <c r="N54" s="32" t="s">
+      <c r="N54" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O54" s="40" t="s">
+      <c r="O54" s="37" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4041,14 +4033,14 @@
         <v>50</v>
       </c>
       <c r="M55" s="4"/>
-      <c r="N55" s="32" t="s">
+      <c r="N55" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O55" s="40" t="s">
+      <c r="O55" s="37" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4084,14 +4076,14 @@
         <v>165</v>
       </c>
       <c r="M56" s="4"/>
-      <c r="N56" s="32" t="s">
+      <c r="N56" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O56" s="40" t="s">
+      <c r="O56" s="37" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4127,14 +4119,14 @@
         <v>171</v>
       </c>
       <c r="M57" s="4"/>
-      <c r="N57" s="32" t="s">
+      <c r="N57" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O57" s="40" t="s">
+      <c r="O57" s="37" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4170,14 +4162,14 @@
         <v>50</v>
       </c>
       <c r="M58" s="4"/>
-      <c r="N58" s="32" t="s">
+      <c r="N58" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O58" s="40" t="s">
+      <c r="O58" s="37" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4213,24 +4205,24 @@
         <v>50</v>
       </c>
       <c r="M59" s="4"/>
-      <c r="N59" s="32" t="s">
+      <c r="N59" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O59" s="40" t="s">
+      <c r="O59" s="37" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="60" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="16">
+    <row r="60" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="15">
         <v>59</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="16" t="s">
         <v>184</v>
       </c>
-      <c r="D60" s="17" t="s">
+      <c r="D60" s="16" t="s">
         <v>185</v>
       </c>
       <c r="E60" s="13">
@@ -4252,31 +4244,28 @@
       <c r="K60" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L60" s="18" t="s">
+      <c r="L60" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="M60" s="18"/>
-      <c r="N60" s="32" t="s">
+      <c r="M60" s="17"/>
+      <c r="N60" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O60" s="40" t="s">
+      <c r="O60" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="P60" s="14"/>
-      <c r="Q60" s="14"/>
-      <c r="R60" s="14"/>
-    </row>
-    <row r="61" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="16">
+    </row>
+    <row r="61" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="15">
         <v>60</v>
       </c>
-      <c r="B61" s="19" t="s">
+      <c r="B61" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="C61" s="17" t="s">
+      <c r="C61" s="16" t="s">
         <v>187</v>
       </c>
-      <c r="D61" s="17" t="s">
+      <c r="D61" s="16" t="s">
         <v>188</v>
       </c>
       <c r="E61" s="13">
@@ -4298,31 +4287,28 @@
       <c r="K61" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="L61" s="18" t="s">
+      <c r="L61" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="M61" s="18"/>
-      <c r="N61" s="32" t="s">
+      <c r="M61" s="17"/>
+      <c r="N61" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O61" s="40" t="s">
+      <c r="O61" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="P61" s="14"/>
-      <c r="Q61" s="14"/>
-      <c r="R61" s="14"/>
-    </row>
-    <row r="62" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="16">
+    </row>
+    <row r="62" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="15">
         <v>61</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B62" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="C62" s="17" t="s">
+      <c r="C62" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="D62" s="17" t="s">
+      <c r="D62" s="16" t="s">
         <v>192</v>
       </c>
       <c r="E62" s="13">
@@ -4344,31 +4330,28 @@
       <c r="K62" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L62" s="18" t="s">
+      <c r="L62" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="M62" s="18"/>
-      <c r="N62" s="32" t="s">
+      <c r="M62" s="17"/>
+      <c r="N62" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O62" s="40" t="s">
+      <c r="O62" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="P62" s="14"/>
-      <c r="Q62" s="14"/>
-      <c r="R62" s="14"/>
-    </row>
-    <row r="63" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="16">
+    </row>
+    <row r="63" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="15">
         <v>62</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C63" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="D63" s="17" t="s">
+      <c r="D63" s="16" t="s">
         <v>195</v>
       </c>
       <c r="E63" s="13">
@@ -4390,31 +4373,28 @@
       <c r="K63" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L63" s="18" t="s">
+      <c r="L63" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="M63" s="18"/>
-      <c r="N63" s="32" t="s">
+      <c r="M63" s="17"/>
+      <c r="N63" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O63" s="40" t="s">
+      <c r="O63" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="P63" s="14"/>
-      <c r="Q63" s="14"/>
-      <c r="R63" s="14"/>
-    </row>
-    <row r="64" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="16">
+    </row>
+    <row r="64" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="15">
         <v>63</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="16" t="s">
         <v>196</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C64" s="16" t="s">
         <v>197</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="D64" s="16" t="s">
         <v>198</v>
       </c>
       <c r="E64" s="13">
@@ -4436,31 +4416,28 @@
       <c r="K64" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L64" s="18" t="s">
+      <c r="L64" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="M64" s="18"/>
-      <c r="N64" s="32" t="s">
+      <c r="M64" s="17"/>
+      <c r="N64" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O64" s="40" t="s">
+      <c r="O64" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="P64" s="14"/>
-      <c r="Q64" s="14"/>
-      <c r="R64" s="14"/>
-    </row>
-    <row r="65" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="16">
+    </row>
+    <row r="65" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="15">
         <v>64</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C65" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>201</v>
       </c>
       <c r="E65" s="13">
@@ -4482,21 +4459,18 @@
       <c r="K65" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L65" s="18" t="s">
+      <c r="L65" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="M65" s="18"/>
-      <c r="N65" s="32" t="s">
+      <c r="M65" s="17"/>
+      <c r="N65" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O65" s="40" t="s">
+      <c r="O65" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="P65" s="14"/>
-      <c r="Q65" s="14"/>
-      <c r="R65" s="14"/>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4532,14 +4506,14 @@
         <v>134</v>
       </c>
       <c r="M66" s="4"/>
-      <c r="N66" s="32" t="s">
+      <c r="N66" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O66" s="40" t="s">
+      <c r="O66" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4574,15 +4548,15 @@
       <c r="L67" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="M67" s="26"/>
-      <c r="N67" s="32" t="s">
+      <c r="M67" s="23"/>
+      <c r="N67" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O67" s="40" t="s">
+      <c r="O67" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4618,14 +4592,14 @@
         <v>50</v>
       </c>
       <c r="M68" s="4"/>
-      <c r="N68" s="32" t="s">
+      <c r="N68" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O68" s="40" t="s">
+      <c r="O68" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -4661,14 +4635,14 @@
         <v>155</v>
       </c>
       <c r="M69" s="4"/>
-      <c r="N69" s="32" t="s">
+      <c r="N69" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O69" s="40" t="s">
+      <c r="O69" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -4704,14 +4678,14 @@
         <v>217</v>
       </c>
       <c r="M70" s="4"/>
-      <c r="N70" s="32" t="s">
+      <c r="N70" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O70" s="40" t="s">
+      <c r="O70" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -4747,14 +4721,14 @@
         <v>50</v>
       </c>
       <c r="M71" s="4"/>
-      <c r="N71" s="32" t="s">
+      <c r="N71" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O71" s="40" t="s">
+      <c r="O71" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -4790,14 +4764,14 @@
         <v>50</v>
       </c>
       <c r="M72" s="4"/>
-      <c r="N72" s="32" t="s">
+      <c r="N72" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O72" s="40" t="s">
+      <c r="O72" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -4825,18 +4799,18 @@
       <c r="K73" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L73" s="18" t="s">
+      <c r="L73" s="17" t="s">
         <v>119</v>
       </c>
       <c r="M73" s="6"/>
-      <c r="N73" s="32" t="s">
+      <c r="N73" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O73" s="40" t="s">
+      <c r="O73" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -4872,14 +4846,14 @@
         <v>50</v>
       </c>
       <c r="M74" s="4"/>
-      <c r="N74" s="32" t="s">
+      <c r="N74" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O74" s="40" t="s">
+      <c r="O74" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -4915,14 +4889,14 @@
         <v>50</v>
       </c>
       <c r="M75" s="4"/>
-      <c r="N75" s="32" t="s">
+      <c r="N75" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O75" s="40" t="s">
+      <c r="O75" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -4958,14 +4932,14 @@
         <v>50</v>
       </c>
       <c r="M76" s="4"/>
-      <c r="N76" s="32" t="s">
+      <c r="N76" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O76" s="40" t="s">
+      <c r="O76" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5001,14 +4975,14 @@
         <v>50</v>
       </c>
       <c r="M77" s="4"/>
-      <c r="N77" s="32" t="s">
+      <c r="N77" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O77" s="40" t="s">
+      <c r="O77" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5044,24 +5018,24 @@
         <v>50</v>
       </c>
       <c r="M78" s="4"/>
-      <c r="N78" s="32" t="s">
+      <c r="N78" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O78" s="40" t="s">
+      <c r="O78" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="79" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
-      <c r="B79" s="19" t="s">
+      <c r="B79" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="C79" s="17" t="s">
+      <c r="C79" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="D79" s="17" t="s">
+      <c r="D79" s="16" t="s">
         <v>237</v>
       </c>
       <c r="E79" s="13">
@@ -5083,25 +5057,22 @@
       <c r="K79" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L79" s="18" t="s">
+      <c r="L79" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="M79" s="18"/>
-      <c r="N79" s="32" t="s">
+      <c r="M79" s="17"/>
+      <c r="N79" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O79" s="40" t="s">
+      <c r="O79" s="37" t="s">
         <v>279</v>
       </c>
-      <c r="P79" s="14"/>
-      <c r="Q79" s="14"/>
-      <c r="R79" s="14"/>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>79</v>
       </c>
-      <c r="B80" s="19" t="s">
+      <c r="B80" s="18" t="s">
         <v>238</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -5132,19 +5103,19 @@
       <c r="L80" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="M80" s="18"/>
-      <c r="N80" s="32" t="s">
+      <c r="M80" s="17"/>
+      <c r="N80" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O80" s="40" t="s">
+      <c r="O80" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>80</v>
       </c>
-      <c r="B81" s="19" t="s">
+      <c r="B81" s="18" t="s">
         <v>241</v>
       </c>
       <c r="C81" s="4" t="s">
@@ -5175,25 +5146,25 @@
       <c r="L81" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="M81" s="18"/>
-      <c r="N81" s="32" t="s">
+      <c r="M81" s="17"/>
+      <c r="N81" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O81" s="40" t="s">
+      <c r="O81" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:18" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
-      <c r="B82" s="19" t="s">
+      <c r="B82" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="C82" s="18" t="s">
+      <c r="C82" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="D82" s="17" t="s">
         <v>246</v>
       </c>
       <c r="E82" s="13">
@@ -5218,22 +5189,19 @@
       <c r="L82" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="M82" s="18"/>
-      <c r="N82" s="32" t="s">
+      <c r="M82" s="17"/>
+      <c r="N82" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O82" s="40" t="s">
+      <c r="O82" s="37" t="s">
         <v>279</v>
       </c>
-      <c r="P82" s="14"/>
-      <c r="Q82" s="14"/>
-      <c r="R82" s="14"/>
-    </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>82</v>
       </c>
-      <c r="B83" s="19" t="s">
+      <c r="B83" s="18" t="s">
         <v>247</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -5264,15 +5232,15 @@
       <c r="L83" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="M83" s="18"/>
-      <c r="N83" s="32" t="s">
+      <c r="M83" s="17"/>
+      <c r="N83" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O83" s="40" t="s">
+      <c r="O83" s="37" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -5308,14 +5276,14 @@
         <v>16</v>
       </c>
       <c r="M84" s="4"/>
-      <c r="N84" s="32" t="s">
+      <c r="N84" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="O84" s="41" t="s">
+      <c r="O84" s="38" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="85" spans="1:18" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -5347,74 +5315,59 @@
       <c r="K85" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L85" s="43" t="s">
+      <c r="L85" s="40" t="s">
         <v>257</v>
       </c>
       <c r="M85" s="4"/>
-      <c r="N85" s="32" t="s">
+      <c r="N85" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="O85" s="41" t="s">
+      <c r="O85" s="38" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="86" spans="1:18" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="20">
+    <row r="86" spans="1:15" ht="56.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="19">
         <v>85</v>
       </c>
-      <c r="B86" s="23" t="s">
+      <c r="B86" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="C86" s="23" t="s">
+      <c r="C86" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="D86" s="23" t="s">
+      <c r="D86" s="20" t="s">
         <v>260</v>
       </c>
-      <c r="E86" s="24">
+      <c r="E86" s="21">
         <v>6</v>
       </c>
-      <c r="F86" s="24">
-        <v>0</v>
-      </c>
-      <c r="G86" s="24">
-        <v>0</v>
-      </c>
-      <c r="H86" s="24"/>
-      <c r="I86" s="24">
+      <c r="F86" s="21">
+        <v>0</v>
+      </c>
+      <c r="G86" s="21">
+        <v>0</v>
+      </c>
+      <c r="H86" s="21"/>
+      <c r="I86" s="21">
         <v>180</v>
       </c>
-      <c r="J86" s="24" t="s">
+      <c r="J86" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="K86" s="34" t="s">
+      <c r="K86" s="31" t="s">
         <v>261</v>
       </c>
-      <c r="L86" s="23" t="s">
+      <c r="L86" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="M86" s="23"/>
-      <c r="N86" s="33" t="s">
+      <c r="M86" s="20"/>
+      <c r="N86" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="O86" s="42" t="s">
+      <c r="O86" s="39" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A87" s="21"/>
-      <c r="B87" s="22"/>
-      <c r="C87" s="22"/>
-      <c r="D87" s="22"/>
-      <c r="E87" s="21"/>
-      <c r="F87" s="21"/>
-      <c r="G87" s="21"/>
-      <c r="H87" s="21"/>
-      <c r="I87" s="21"/>
-      <c r="J87" s="21"/>
-      <c r="K87" s="21"/>
-      <c r="L87" s="22"/>
-      <c r="M87" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L50">
@@ -5482,6 +5435,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="07db5020-ba8e-48bf-aa17-fbace2a70736">
+      <UserInfo>
+        <DisplayName>CAP K24T-TEAM01 Members</DisplayName>
+        <AccountId>17</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A95A7398140C45A2F719D38434B23A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8f464c4684f4805cd2f27ee87272a526">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07db5020-ba8e-48bf-aa17-fbace2a70736" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1a8c984c74c8b52243a5f41979946bd" ns2:_="">
     <xsd:import namespace="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
@@ -5629,20 +5596,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="07db5020-ba8e-48bf-aa17-fbace2a70736">
-      <UserInfo>
-        <DisplayName>CAP K24T-TEAM01 Members</DisplayName>
-        <AccountId>17</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
   <ds:schemaRefs>
@@ -5652,6 +5605,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{179DDC9E-E391-4AD2-A488-D9C201286EF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648878AA-48B2-4081-A1D0-3EB795A895EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5667,14 +5630,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{179DDC9E-E391-4AD2-A488-D9C201286EF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Starting to do View study program user story
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E32EAC7-7E6D-4662-A02B-402B3FBBBF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB6FED-ACA0-47F4-B21A-E1CBFF637347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="280">
   <si>
     <t>STT</t>
   </si>
@@ -870,9 +870,6 @@
   </si>
   <si>
     <t>Cơ sở ngành</t>
-  </si>
-  <si>
-    <t>Chuyên ngành</t>
   </si>
   <si>
     <t>Chuyên ngành Công nghệ Phần mềm</t>
@@ -1703,8 +1700,8 @@
   <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3779,7 +3776,7 @@
         <v>264</v>
       </c>
       <c r="O49" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
@@ -3822,7 +3819,7 @@
         <v>264</v>
       </c>
       <c r="O50" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
@@ -3865,7 +3862,7 @@
         <v>264</v>
       </c>
       <c r="O51" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
@@ -3908,7 +3905,7 @@
         <v>264</v>
       </c>
       <c r="O52" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
@@ -3951,7 +3948,7 @@
         <v>264</v>
       </c>
       <c r="O53" s="37" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -3994,7 +3991,7 @@
         <v>265</v>
       </c>
       <c r="O54" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -4037,7 +4034,7 @@
         <v>265</v>
       </c>
       <c r="O55" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -4080,7 +4077,7 @@
         <v>265</v>
       </c>
       <c r="O56" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
@@ -4123,7 +4120,7 @@
         <v>265</v>
       </c>
       <c r="O57" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -4166,7 +4163,7 @@
         <v>265</v>
       </c>
       <c r="O58" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -4209,7 +4206,7 @@
         <v>265</v>
       </c>
       <c r="O59" s="37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="60" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -4252,7 +4249,7 @@
         <v>266</v>
       </c>
       <c r="O60" s="37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -4295,7 +4292,7 @@
         <v>266</v>
       </c>
       <c r="O61" s="37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="62" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -4338,7 +4335,7 @@
         <v>266</v>
       </c>
       <c r="O62" s="37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="63" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -4381,7 +4378,7 @@
         <v>266</v>
       </c>
       <c r="O63" s="37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="64" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -4424,7 +4421,7 @@
         <v>266</v>
       </c>
       <c r="O64" s="37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -4467,7 +4464,7 @@
         <v>266</v>
       </c>
       <c r="O65" s="37" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.3">
@@ -4510,7 +4507,7 @@
         <v>267</v>
       </c>
       <c r="O66" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.3">
@@ -4553,7 +4550,7 @@
         <v>267</v>
       </c>
       <c r="O67" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
@@ -4596,7 +4593,7 @@
         <v>267</v>
       </c>
       <c r="O68" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.3">
@@ -4639,7 +4636,7 @@
         <v>267</v>
       </c>
       <c r="O69" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.3">
@@ -4682,7 +4679,7 @@
         <v>267</v>
       </c>
       <c r="O70" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.3">
@@ -4725,7 +4722,7 @@
         <v>267</v>
       </c>
       <c r="O71" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.3">
@@ -4768,7 +4765,7 @@
         <v>267</v>
       </c>
       <c r="O72" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.3">
@@ -4807,7 +4804,7 @@
         <v>267</v>
       </c>
       <c r="O73" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.3">
@@ -4850,7 +4847,7 @@
         <v>267</v>
       </c>
       <c r="O74" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
@@ -4893,7 +4890,7 @@
         <v>267</v>
       </c>
       <c r="O75" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
@@ -4936,7 +4933,7 @@
         <v>267</v>
       </c>
       <c r="O76" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
@@ -4979,7 +4976,7 @@
         <v>267</v>
       </c>
       <c r="O77" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
@@ -5022,7 +5019,7 @@
         <v>267</v>
       </c>
       <c r="O78" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5065,7 +5062,7 @@
         <v>267</v>
       </c>
       <c r="O79" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
@@ -5108,7 +5105,7 @@
         <v>267</v>
       </c>
       <c r="O80" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
@@ -5151,7 +5148,7 @@
         <v>267</v>
       </c>
       <c r="O81" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="82" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5194,7 +5191,7 @@
         <v>267</v>
       </c>
       <c r="O82" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
@@ -5237,7 +5234,7 @@
         <v>267</v>
       </c>
       <c r="O83" s="37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
@@ -5280,7 +5277,7 @@
         <v>10</v>
       </c>
       <c r="O84" s="38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="28.2" x14ac:dyDescent="0.3">
@@ -5323,10 +5320,10 @@
         <v>10</v>
       </c>
       <c r="O85" s="38" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="86" spans="1:15" ht="56.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="19">
         <v>85</v>
       </c>
@@ -5366,57 +5363,57 @@
         <v>10</v>
       </c>
       <c r="O86" s="39" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L50">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:J47">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>$K46&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:M47 B73:K73 M73 B74:M86 B48:M72 B2:M45 N2:N86">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:C86 B2:C45">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L70 L67 B61:B65 B79:B83">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="4" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50 L73 L53">
-    <cfRule type="expression" dxfId="3" priority="9">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>#REF!&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:J47">
-    <cfRule type="expression" dxfId="2" priority="10">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:C47">
-    <cfRule type="expression" dxfId="1" priority="11">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O86">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update major knowledge group row
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FB6FED-ACA0-47F4-B21A-E1CBFF637347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC746DB5-F0B5-4689-9946-B4920E3F53A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -1215,7 +1215,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1700,8 +1714,8 @@
   <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P54" sqref="P54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5368,52 +5382,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L50">
-    <cfRule type="expression" dxfId="9" priority="6">
+    <cfRule type="expression" dxfId="11" priority="8">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="10" priority="7">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:J47">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="9" priority="6">
       <formula>$K46&lt;&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K46:M47 B73:K73 M73 B74:M86 B48:M72 B2:M45 N2:N86">
-    <cfRule type="expression" dxfId="6" priority="7">
+  <conditionalFormatting sqref="K46:M47 B73:K73 M73 B74:M86 B48:M72 B2:M45 N3:N86">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:C86 B2:C45">
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L70 L67 B61:B65 B79:B83">
-    <cfRule type="expression" dxfId="4" priority="9">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50 L73 L53">
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>#REF!&gt;=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:J47">
-    <cfRule type="expression" dxfId="2" priority="11">
+    <cfRule type="expression" dxfId="4" priority="13">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46:C47">
-    <cfRule type="expression" dxfId="1" priority="12">
+    <cfRule type="expression" dxfId="3" priority="14">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O86">
-    <cfRule type="expression" dxfId="0" priority="2">
+  <conditionalFormatting sqref="O3:O86">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>#REF!=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>#REF!=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Complete View study program
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC746DB5-F0B5-4689-9946-B4920E3F53A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA98F43-A6BB-471C-A3EF-060254570741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -860,31 +860,31 @@
     <t>Mã loại kiến thức</t>
   </si>
   <si>
-    <t>Đại cương</t>
-  </si>
-  <si>
     <t>DCKTL</t>
   </si>
   <si>
-    <t>Đại cương không tích luỹ</t>
-  </si>
-  <si>
-    <t>Cơ sở ngành</t>
-  </si>
-  <si>
-    <t>Chuyên ngành Công nghệ Phần mềm</t>
-  </si>
-  <si>
-    <t>Chuyên ngành Công nghệ Dữ liệu</t>
-  </si>
-  <si>
-    <t>Chuyên ngành An ninh Mạng và IoT</t>
-  </si>
-  <si>
-    <t>Các môn tự chọn chuyên ngành</t>
-  </si>
-  <si>
     <t>Thực tập tốt nghiệp/Khóa luận - Đồ án tốt nghiệp/Học phần tốt nghiệp</t>
+  </si>
+  <si>
+    <t>Kiến thức cơ sở ngành (36 tín chỉ = 18 bắt buộc + 18 tự chọn )</t>
+  </si>
+  <si>
+    <t>Chuyên ngành Công nghệ Phần mềm (18 tín chỉ  bắt buộc)</t>
+  </si>
+  <si>
+    <t>Chuyên ngành An ninh Mạng và IoT (18 tín chỉ)</t>
+  </si>
+  <si>
+    <t>Các môn tự chọn chuyên ngành (6 tín chỉ)</t>
+  </si>
+  <si>
+    <t>Đại cương (61 TC tích luỹ)</t>
+  </si>
+  <si>
+    <t>Đại cương không tích luỹ (15 TC không tích luỹ)</t>
+  </si>
+  <si>
+    <t>Chuyên ngành Công nghệ Dữ liệu (18 tín chỉ bắt buộc)</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1199,17 +1199,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1713,9 +1710,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE44191-4F7D-454A-9855-FE690642DDD6}">
   <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1818,8 +1815,8 @@
       <c r="N2" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O2" s="37" t="s">
-        <v>271</v>
+      <c r="O2" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1859,8 +1856,8 @@
       <c r="N3" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O3" s="37" t="s">
-        <v>271</v>
+      <c r="O3" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -1900,8 +1897,8 @@
       <c r="N4" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O4" s="37" t="s">
-        <v>271</v>
+      <c r="O4" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1941,8 +1938,8 @@
       <c r="N5" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O5" s="37" t="s">
-        <v>271</v>
+      <c r="O5" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1982,8 +1979,8 @@
       <c r="N6" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O6" s="37" t="s">
-        <v>271</v>
+      <c r="O6" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
@@ -2023,8 +2020,8 @@
       <c r="N7" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O7" s="37" t="s">
-        <v>271</v>
+      <c r="O7" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -2062,8 +2059,8 @@
       <c r="N8" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O8" s="37" t="s">
-        <v>271</v>
+      <c r="O8" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -2101,8 +2098,8 @@
       <c r="N9" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O9" s="37" t="s">
-        <v>271</v>
+      <c r="O9" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -2140,8 +2137,8 @@
       <c r="N10" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O10" s="37" t="s">
-        <v>271</v>
+      <c r="O10" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -2179,8 +2176,8 @@
       <c r="N11" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O11" s="37" t="s">
-        <v>271</v>
+      <c r="O11" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -2218,8 +2215,8 @@
       <c r="N12" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O12" s="37" t="s">
-        <v>271</v>
+      <c r="O12" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -2257,8 +2254,8 @@
       <c r="N13" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O13" s="37" t="s">
-        <v>271</v>
+      <c r="O13" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -2298,8 +2295,8 @@
       <c r="N14" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O14" s="37" t="s">
-        <v>271</v>
+      <c r="O14" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -2339,8 +2336,8 @@
       <c r="N15" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O15" s="37" t="s">
-        <v>271</v>
+      <c r="O15" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -2382,8 +2379,8 @@
       <c r="N16" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O16" s="37" t="s">
-        <v>271</v>
+      <c r="O16" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -2425,8 +2422,8 @@
       <c r="N17" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O17" s="37" t="s">
-        <v>271</v>
+      <c r="O17" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -2468,8 +2465,8 @@
       <c r="N18" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O18" s="37" t="s">
-        <v>271</v>
+      <c r="O18" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -2511,8 +2508,8 @@
       <c r="N19" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O19" s="37" t="s">
-        <v>271</v>
+      <c r="O19" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -2554,8 +2551,8 @@
       <c r="N20" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O20" s="37" t="s">
-        <v>271</v>
+      <c r="O20" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -2597,8 +2594,8 @@
       <c r="N21" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O21" s="37" t="s">
-        <v>271</v>
+      <c r="O21" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -2640,8 +2637,8 @@
       <c r="N22" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O22" s="37" t="s">
-        <v>271</v>
+      <c r="O22" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -2683,8 +2680,8 @@
       <c r="N23" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O23" s="37" t="s">
-        <v>271</v>
+      <c r="O23" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2726,8 +2723,8 @@
       <c r="N24" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O24" s="37" t="s">
-        <v>271</v>
+      <c r="O24" s="38" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -2769,11 +2766,11 @@
       <c r="N25" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="O25" s="37" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O25" s="38" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="32">
         <v>25</v>
       </c>
@@ -2808,13 +2805,13 @@
       </c>
       <c r="M26" s="24"/>
       <c r="N26" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="O26" s="37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="O26" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A27" s="32">
         <v>26</v>
       </c>
@@ -2849,13 +2846,13 @@
       </c>
       <c r="M27" s="24"/>
       <c r="N27" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="O27" s="37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="O27" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A28" s="32">
         <v>27</v>
       </c>
@@ -2890,13 +2887,13 @@
       </c>
       <c r="M28" s="27"/>
       <c r="N28" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="O28" s="37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="O28" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="32">
         <v>28</v>
       </c>
@@ -2931,13 +2928,13 @@
       </c>
       <c r="M29" s="27"/>
       <c r="N29" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="O29" s="37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="O29" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="32">
         <v>29</v>
       </c>
@@ -2970,13 +2967,13 @@
       <c r="L30" s="27"/>
       <c r="M30" s="27"/>
       <c r="N30" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="O30" s="37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="O30" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="32">
         <v>30</v>
       </c>
@@ -3009,13 +3006,13 @@
       <c r="L31" s="27"/>
       <c r="M31" s="27"/>
       <c r="N31" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="O31" s="37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+      <c r="O31" s="38" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3054,11 +3051,11 @@
       <c r="N32" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O32" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O32" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3097,11 +3094,11 @@
       <c r="N33" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O33" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O33" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3140,11 +3137,11 @@
       <c r="N34" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O34" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O34" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -3183,11 +3180,11 @@
       <c r="N35" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O35" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O35" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -3226,11 +3223,11 @@
       <c r="N36" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O36" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O36" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -3269,11 +3266,11 @@
       <c r="N37" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O37" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O37" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -3312,11 +3309,11 @@
       <c r="N38" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O38" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O38" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -3355,11 +3352,11 @@
       <c r="N39" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O39" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O39" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -3398,11 +3395,11 @@
       <c r="N40" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O40" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O40" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -3441,11 +3438,11 @@
       <c r="N41" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O41" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O41" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -3484,11 +3481,11 @@
       <c r="N42" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O42" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O42" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -3527,11 +3524,11 @@
       <c r="N43" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O43" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O43" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -3570,11 +3567,11 @@
       <c r="N44" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O44" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O44" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -3613,11 +3610,11 @@
       <c r="N45" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O45" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O45" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -3658,11 +3655,11 @@
       <c r="N46" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O46" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O46" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -3703,11 +3700,11 @@
       <c r="N47" s="29" t="s">
         <v>263</v>
       </c>
-      <c r="O47" s="37" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O47" s="38" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -3746,11 +3743,11 @@
       <c r="N48" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O48" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O48" s="38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -3789,11 +3786,11 @@
       <c r="N49" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O49" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O49" s="38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -3832,11 +3829,11 @@
       <c r="N50" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O50" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O50" s="38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -3875,11 +3872,11 @@
       <c r="N51" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O51" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O51" s="38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -3918,11 +3915,11 @@
       <c r="N52" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O52" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O52" s="38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -3961,11 +3958,11 @@
       <c r="N53" s="29" t="s">
         <v>264</v>
       </c>
-      <c r="O53" s="37" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O53" s="38" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4004,11 +4001,11 @@
       <c r="N54" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O54" s="37" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O54" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4047,11 +4044,11 @@
       <c r="N55" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O55" s="37" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O55" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4090,11 +4087,11 @@
       <c r="N56" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O56" s="37" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O56" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4133,11 +4130,11 @@
       <c r="N57" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O57" s="37" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O57" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4176,11 +4173,11 @@
       <c r="N58" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O58" s="37" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O58" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4219,11 +4216,11 @@
       <c r="N59" s="29" t="s">
         <v>265</v>
       </c>
-      <c r="O59" s="37" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O59" s="38" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A60" s="15">
         <v>59</v>
       </c>
@@ -4262,11 +4259,11 @@
       <c r="N60" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O60" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O60" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A61" s="15">
         <v>60</v>
       </c>
@@ -4305,11 +4302,11 @@
       <c r="N61" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O61" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O61" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A62" s="15">
         <v>61</v>
       </c>
@@ -4348,11 +4345,11 @@
       <c r="N62" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O62" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O62" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A63" s="15">
         <v>62</v>
       </c>
@@ -4391,11 +4388,11 @@
       <c r="N63" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O63" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O63" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A64" s="15">
         <v>63</v>
       </c>
@@ -4434,11 +4431,11 @@
       <c r="N64" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O64" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="65" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O64" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A65" s="15">
         <v>64</v>
       </c>
@@ -4477,11 +4474,11 @@
       <c r="N65" s="29" t="s">
         <v>266</v>
       </c>
-      <c r="O65" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O65" s="38" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -4520,11 +4517,11 @@
       <c r="N66" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O66" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O66" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -4563,11 +4560,11 @@
       <c r="N67" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O67" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O67" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -4606,11 +4603,11 @@
       <c r="N68" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O68" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O68" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -4649,11 +4646,11 @@
       <c r="N69" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O69" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O69" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -4692,11 +4689,11 @@
       <c r="N70" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O70" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O70" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -4735,11 +4732,11 @@
       <c r="N71" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O71" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O71" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -4778,11 +4775,11 @@
       <c r="N72" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O72" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O72" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -4817,11 +4814,11 @@
       <c r="N73" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O73" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O73" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -4860,11 +4857,11 @@
       <c r="N74" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O74" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O74" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -4903,11 +4900,11 @@
       <c r="N75" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O75" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O75" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -4946,11 +4943,11 @@
       <c r="N76" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O76" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O76" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -4989,11 +4986,11 @@
       <c r="N77" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O77" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O77" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5032,11 +5029,11 @@
       <c r="N78" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O78" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O78" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -5075,11 +5072,11 @@
       <c r="N79" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O79" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O79" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -5118,11 +5115,11 @@
       <c r="N80" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O80" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O80" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -5161,11 +5158,11 @@
       <c r="N81" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O81" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O81" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -5204,11 +5201,11 @@
       <c r="N82" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O82" s="37" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O82" s="38" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -5247,8 +5244,8 @@
       <c r="N83" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="O83" s="37" t="s">
-        <v>278</v>
+      <c r="O83" s="38" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="27.6" x14ac:dyDescent="0.3">
@@ -5291,7 +5288,7 @@
         <v>10</v>
       </c>
       <c r="O84" s="38" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="28.2" x14ac:dyDescent="0.3">
@@ -5326,7 +5323,7 @@
       <c r="K85" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L85" s="40" t="s">
+      <c r="L85" s="37" t="s">
         <v>257</v>
       </c>
       <c r="M85" s="4"/>
@@ -5334,7 +5331,7 @@
         <v>10</v>
       </c>
       <c r="O85" s="38" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="42.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -5377,7 +5374,7 @@
         <v>10</v>
       </c>
       <c r="O86" s="39" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>
@@ -5426,7 +5423,7 @@
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O86">
+  <conditionalFormatting sqref="O26:O86">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>#REF!=1</formula>
     </cfRule>
@@ -5436,7 +5433,7 @@
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2">
+  <conditionalFormatting sqref="O2:O25">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF!=1</formula>
     </cfRule>
@@ -5447,15 +5444,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="07db5020-ba8e-48bf-aa17-fbace2a70736">
@@ -5469,7 +5457,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A95A7398140C45A2F719D38434B23A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8f464c4684f4805cd2f27ee87272a526">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07db5020-ba8e-48bf-aa17-fbace2a70736" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1a8c984c74c8b52243a5f41979946bd" ns2:_="">
     <xsd:import namespace="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
@@ -5617,15 +5605,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{179DDC9E-E391-4AD2-A488-D9C201286EF9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5635,7 +5624,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648878AA-48B2-4081-A1D0-3EB795A895EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5651,4 +5640,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update import study program and view study program after fixing datatabase
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA98F43-A6BB-471C-A3EF-060254570741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF3AAC5-F5E1-4689-9EDD-CE1F9ECC6298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -1711,8 +1711,8 @@
   <dimension ref="A1:O86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J56" sqref="J56"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5458,6 +5458,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010020A95A7398140C45A2F719D38434B23A" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8f464c4684f4805cd2f27ee87272a526">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="07db5020-ba8e-48bf-aa17-fbace2a70736" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b1a8c984c74c8b52243a5f41979946bd" ns2:_="">
     <xsd:import namespace="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
@@ -5605,15 +5614,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{179DDC9E-E391-4AD2-A488-D9C201286EF9}">
   <ds:schemaRefs>
@@ -5625,6 +5625,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{648878AA-48B2-4081-A1D0-3EB795A895EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5640,12 +5648,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update view study program
</commit_message>
<xml_diff>
--- a/StudyProgressManagement/Uploads/CTDT_Test.xlsx
+++ b/StudyProgressManagement/Uploads/CTDT_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Desktop\StudyProgram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13D8FE0-3897-4CEA-89D5-E090CBD92E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF8BE3B-A62E-4525-89CB-248232B9CA12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6C2B6FC-ED23-41F9-89D8-E92A8C2587DC}"/>
   </bookViews>
@@ -866,31 +866,31 @@
     <t>Thực tập tốt nghiệp/Khóa luận - Đồ án tốt nghiệp/Học phần tốt nghiệp</t>
   </si>
   <si>
-    <t>Kiến thức cơ sở ngành (36 tín chỉ = 18 bắt buộc + 18 tự chọn )</t>
-  </si>
-  <si>
-    <t>Chuyên ngành Công nghệ Phần mềm (18 tín chỉ  bắt buộc)</t>
-  </si>
-  <si>
-    <t>Chuyên ngành An ninh Mạng và IoT (18 tín chỉ)</t>
-  </si>
-  <si>
-    <t>Các môn tự chọn chuyên ngành (6 tín chỉ)</t>
-  </si>
-  <si>
-    <t>Đại cương (61 TC tích luỹ)</t>
-  </si>
-  <si>
-    <t>Đại cương không tích luỹ (15 TC không tích luỹ)</t>
-  </si>
-  <si>
-    <t>Chuyên ngành Công nghệ Dữ liệu (18 tín chỉ bắt buộc)</t>
-  </si>
-  <si>
     <t>Số chỉ BB</t>
   </si>
   <si>
     <t>Số chỉ TC</t>
+  </si>
+  <si>
+    <t>Đại cương</t>
+  </si>
+  <si>
+    <t>Đại cương không tích luỹ</t>
+  </si>
+  <si>
+    <t>Kiến thức cơ sở ngành</t>
+  </si>
+  <si>
+    <t>Chuyên ngành Công nghệ Phần mềm</t>
+  </si>
+  <si>
+    <t>Chuyên ngành Công nghệ Dữ liệu</t>
+  </si>
+  <si>
+    <t>Chuyên ngành An ninh Mạng và IoT</t>
+  </si>
+  <si>
+    <t>Các môn tự chọn chuyên ngành</t>
   </si>
 </sst>
 </file>
@@ -1599,8 +1599,8 @@
   <dimension ref="A1:Q86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O20" sqref="O20"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1667,10 +1667,10 @@
         <v>269</v>
       </c>
       <c r="P1" s="26" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="Q1" s="26" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1711,7 +1711,7 @@
         <v>262</v>
       </c>
       <c r="O2" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P2" s="32">
         <v>61</v>
@@ -1756,7 +1756,7 @@
         <v>262</v>
       </c>
       <c r="O3" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P3" s="32">
         <v>61</v>
@@ -1801,7 +1801,7 @@
         <v>262</v>
       </c>
       <c r="O4" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P4" s="32">
         <v>61</v>
@@ -1846,7 +1846,7 @@
         <v>262</v>
       </c>
       <c r="O5" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P5" s="32">
         <v>61</v>
@@ -1891,7 +1891,7 @@
         <v>262</v>
       </c>
       <c r="O6" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P6" s="32">
         <v>61</v>
@@ -1936,7 +1936,7 @@
         <v>262</v>
       </c>
       <c r="O7" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P7" s="32">
         <v>61</v>
@@ -1979,7 +1979,7 @@
         <v>262</v>
       </c>
       <c r="O8" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P8" s="32">
         <v>61</v>
@@ -2022,7 +2022,7 @@
         <v>262</v>
       </c>
       <c r="O9" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P9" s="32">
         <v>61</v>
@@ -2065,7 +2065,7 @@
         <v>262</v>
       </c>
       <c r="O10" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P10" s="32">
         <v>61</v>
@@ -2108,7 +2108,7 @@
         <v>262</v>
       </c>
       <c r="O11" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P11" s="32">
         <v>61</v>
@@ -2151,7 +2151,7 @@
         <v>262</v>
       </c>
       <c r="O12" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P12" s="32">
         <v>61</v>
@@ -2194,7 +2194,7 @@
         <v>262</v>
       </c>
       <c r="O13" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P13" s="32">
         <v>61</v>
@@ -2239,7 +2239,7 @@
         <v>262</v>
       </c>
       <c r="O14" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P14" s="32">
         <v>61</v>
@@ -2284,7 +2284,7 @@
         <v>262</v>
       </c>
       <c r="O15" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P15" s="32">
         <v>61</v>
@@ -2331,7 +2331,7 @@
         <v>262</v>
       </c>
       <c r="O16" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P16" s="32">
         <v>61</v>
@@ -2378,7 +2378,7 @@
         <v>262</v>
       </c>
       <c r="O17" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P17" s="32">
         <v>61</v>
@@ -2425,7 +2425,7 @@
         <v>262</v>
       </c>
       <c r="O18" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P18" s="32">
         <v>61</v>
@@ -2472,7 +2472,7 @@
         <v>262</v>
       </c>
       <c r="O19" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P19" s="32">
         <v>61</v>
@@ -2519,7 +2519,7 @@
         <v>262</v>
       </c>
       <c r="O20" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P20" s="32">
         <v>61</v>
@@ -2566,7 +2566,7 @@
         <v>262</v>
       </c>
       <c r="O21" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P21" s="32">
         <v>61</v>
@@ -2613,7 +2613,7 @@
         <v>262</v>
       </c>
       <c r="O22" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P22" s="32">
         <v>61</v>
@@ -2660,7 +2660,7 @@
         <v>262</v>
       </c>
       <c r="O23" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P23" s="32">
         <v>61</v>
@@ -2707,7 +2707,7 @@
         <v>262</v>
       </c>
       <c r="O24" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P24" s="32">
         <v>61</v>
@@ -2754,14 +2754,14 @@
         <v>262</v>
       </c>
       <c r="O25" s="33" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="P25" s="32">
         <v>61</v>
       </c>
       <c r="Q25" s="24"/>
     </row>
-    <row r="26" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="21">
         <v>25</v>
       </c>
@@ -2799,14 +2799,14 @@
         <v>271</v>
       </c>
       <c r="O26" s="28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P26" s="24">
         <v>15</v>
       </c>
       <c r="Q26" s="24"/>
     </row>
-    <row r="27" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
         <v>26</v>
       </c>
@@ -2844,14 +2844,14 @@
         <v>271</v>
       </c>
       <c r="O27" s="28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P27" s="24">
         <v>15</v>
       </c>
       <c r="Q27" s="24"/>
     </row>
-    <row r="28" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
         <v>27</v>
       </c>
@@ -2889,14 +2889,14 @@
         <v>271</v>
       </c>
       <c r="O28" s="28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P28" s="24">
         <v>15</v>
       </c>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="21">
         <v>28</v>
       </c>
@@ -2934,14 +2934,14 @@
         <v>271</v>
       </c>
       <c r="O29" s="28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P29" s="24">
         <v>15</v>
       </c>
       <c r="Q29" s="24"/>
     </row>
-    <row r="30" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="21">
         <v>29</v>
       </c>
@@ -2977,14 +2977,14 @@
         <v>271</v>
       </c>
       <c r="O30" s="28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P30" s="24">
         <v>15</v>
       </c>
       <c r="Q30" s="24"/>
     </row>
-    <row r="31" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
         <v>30</v>
       </c>
@@ -3020,14 +3020,14 @@
         <v>271</v>
       </c>
       <c r="O31" s="28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P31" s="24">
         <v>15</v>
       </c>
       <c r="Q31" s="24"/>
     </row>
-    <row r="32" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>263</v>
       </c>
       <c r="O32" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P32" s="24">
         <v>18</v>
@@ -3076,7 +3076,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>263</v>
       </c>
       <c r="O33" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P33" s="24">
         <v>18</v>
@@ -3125,7 +3125,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>263</v>
       </c>
       <c r="O34" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P34" s="24">
         <v>18</v>
@@ -3174,7 +3174,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>263</v>
       </c>
       <c r="O35" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P35" s="24">
         <v>18</v>
@@ -3223,7 +3223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>263</v>
       </c>
       <c r="O36" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P36" s="24">
         <v>18</v>
@@ -3272,7 +3272,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>263</v>
       </c>
       <c r="O37" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P37" s="24">
         <v>18</v>
@@ -3321,7 +3321,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -3361,7 +3361,7 @@
         <v>263</v>
       </c>
       <c r="O38" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P38" s="24">
         <v>18</v>
@@ -3370,7 +3370,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -3410,7 +3410,7 @@
         <v>263</v>
       </c>
       <c r="O39" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P39" s="24">
         <v>18</v>
@@ -3419,7 +3419,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>263</v>
       </c>
       <c r="O40" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P40" s="24">
         <v>18</v>
@@ -3468,7 +3468,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>263</v>
       </c>
       <c r="O41" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P41" s="24">
         <v>18</v>
@@ -3517,7 +3517,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>263</v>
       </c>
       <c r="O42" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P42" s="24">
         <v>18</v>
@@ -3566,7 +3566,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>263</v>
       </c>
       <c r="O43" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P43" s="24">
         <v>18</v>
@@ -3615,7 +3615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>263</v>
       </c>
       <c r="O44" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P44" s="24">
         <v>18</v>
@@ -3664,7 +3664,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>263</v>
       </c>
       <c r="O45" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P45" s="24">
         <v>18</v>
@@ -3713,7 +3713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>263</v>
       </c>
       <c r="O46" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P46" s="24">
         <v>18</v>
@@ -3764,7 +3764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>263</v>
       </c>
       <c r="O47" s="28" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="P47" s="24">
         <v>18</v>
@@ -3815,7 +3815,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -3855,14 +3855,14 @@
         <v>264</v>
       </c>
       <c r="O48" s="28" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="P48" s="24">
         <v>18</v>
       </c>
       <c r="Q48" s="24"/>
     </row>
-    <row r="49" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -3902,14 +3902,14 @@
         <v>264</v>
       </c>
       <c r="O49" s="28" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="P49" s="24">
         <v>18</v>
       </c>
       <c r="Q49" s="24"/>
     </row>
-    <row r="50" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -3949,14 +3949,14 @@
         <v>264</v>
       </c>
       <c r="O50" s="28" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="P50" s="24">
         <v>18</v>
       </c>
       <c r="Q50" s="24"/>
     </row>
-    <row r="51" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -3996,14 +3996,14 @@
         <v>264</v>
       </c>
       <c r="O51" s="28" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="P51" s="24">
         <v>18</v>
       </c>
       <c r="Q51" s="24"/>
     </row>
-    <row r="52" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -4043,14 +4043,14 @@
         <v>264</v>
       </c>
       <c r="O52" s="28" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="P52" s="24">
         <v>18</v>
       </c>
       <c r="Q52" s="24"/>
     </row>
-    <row r="53" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -4090,14 +4090,14 @@
         <v>264</v>
       </c>
       <c r="O53" s="28" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="P53" s="24">
         <v>18</v>
       </c>
       <c r="Q53" s="24"/>
     </row>
-    <row r="54" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -4144,7 +4144,7 @@
       </c>
       <c r="Q54" s="24"/>
     </row>
-    <row r="55" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -4191,7 +4191,7 @@
       </c>
       <c r="Q55" s="24"/>
     </row>
-    <row r="56" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -4238,7 +4238,7 @@
       </c>
       <c r="Q56" s="24"/>
     </row>
-    <row r="57" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -4285,7 +4285,7 @@
       </c>
       <c r="Q57" s="24"/>
     </row>
-    <row r="58" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="Q58" s="24"/>
     </row>
-    <row r="59" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -4379,7 +4379,7 @@
       </c>
       <c r="Q59" s="24"/>
     </row>
-    <row r="60" spans="1:17" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -4419,14 +4419,14 @@
         <v>266</v>
       </c>
       <c r="O60" s="28" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="P60" s="24">
         <v>18</v>
       </c>
       <c r="Q60" s="24"/>
     </row>
-    <row r="61" spans="1:17" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12">
         <v>60</v>
       </c>
@@ -4466,14 +4466,14 @@
         <v>266</v>
       </c>
       <c r="O61" s="28" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="P61" s="24">
         <v>18</v>
       </c>
       <c r="Q61" s="24"/>
     </row>
-    <row r="62" spans="1:17" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12">
         <v>61</v>
       </c>
@@ -4513,14 +4513,14 @@
         <v>266</v>
       </c>
       <c r="O62" s="28" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="P62" s="24">
         <v>18</v>
       </c>
       <c r="Q62" s="24"/>
     </row>
-    <row r="63" spans="1:17" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>62</v>
       </c>
@@ -4560,14 +4560,14 @@
         <v>266</v>
       </c>
       <c r="O63" s="28" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="P63" s="24">
         <v>18</v>
       </c>
       <c r="Q63" s="24"/>
     </row>
-    <row r="64" spans="1:17" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12">
         <v>63</v>
       </c>
@@ -4607,14 +4607,14 @@
         <v>266</v>
       </c>
       <c r="O64" s="28" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="P64" s="24">
         <v>18</v>
       </c>
       <c r="Q64" s="24"/>
     </row>
-    <row r="65" spans="1:17" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12">
         <v>64</v>
       </c>
@@ -4654,14 +4654,14 @@
         <v>266</v>
       </c>
       <c r="O65" s="28" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="P65" s="24">
         <v>18</v>
       </c>
       <c r="Q65" s="24"/>
     </row>
-    <row r="66" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -4701,14 +4701,14 @@
         <v>267</v>
       </c>
       <c r="O66" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P66" s="24"/>
       <c r="Q66" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -4748,14 +4748,14 @@
         <v>267</v>
       </c>
       <c r="O67" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P67" s="24"/>
       <c r="Q67" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -4795,14 +4795,14 @@
         <v>267</v>
       </c>
       <c r="O68" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P68" s="24"/>
       <c r="Q68" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -4842,14 +4842,14 @@
         <v>267</v>
       </c>
       <c r="O69" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P69" s="24"/>
       <c r="Q69" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -4889,14 +4889,14 @@
         <v>267</v>
       </c>
       <c r="O70" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P70" s="24"/>
       <c r="Q70" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -4936,14 +4936,14 @@
         <v>267</v>
       </c>
       <c r="O71" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P71" s="24"/>
       <c r="Q71" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -4983,14 +4983,14 @@
         <v>267</v>
       </c>
       <c r="O72" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P72" s="24"/>
       <c r="Q72" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -5026,14 +5026,14 @@
         <v>267</v>
       </c>
       <c r="O73" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P73" s="24"/>
       <c r="Q73" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -5073,14 +5073,14 @@
         <v>267</v>
       </c>
       <c r="O74" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P74" s="24"/>
       <c r="Q74" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -5120,14 +5120,14 @@
         <v>267</v>
       </c>
       <c r="O75" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P75" s="24"/>
       <c r="Q75" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -5167,14 +5167,14 @@
         <v>267</v>
       </c>
       <c r="O76" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P76" s="24"/>
       <c r="Q76" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -5214,14 +5214,14 @@
         <v>267</v>
       </c>
       <c r="O77" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P77" s="24"/>
       <c r="Q77" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -5261,14 +5261,14 @@
         <v>267</v>
       </c>
       <c r="O78" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P78" s="24"/>
       <c r="Q78" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:17" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -5308,14 +5308,14 @@
         <v>267</v>
       </c>
       <c r="O79" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P79" s="24"/>
       <c r="Q79" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -5355,14 +5355,14 @@
         <v>267</v>
       </c>
       <c r="O80" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P80" s="24"/>
       <c r="Q80" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -5402,14 +5402,14 @@
         <v>267</v>
       </c>
       <c r="O81" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P81" s="24"/>
       <c r="Q81" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:17" s="13" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -5449,14 +5449,14 @@
         <v>267</v>
       </c>
       <c r="O82" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P82" s="24"/>
       <c r="Q82" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>267</v>
       </c>
       <c r="O83" s="28" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="P83" s="24"/>
       <c r="Q83" s="24">
@@ -5707,12 +5707,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O25">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:Q86">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5870,15 +5870,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="07db5020-ba8e-48bf-aa17-fbace2a70736">
@@ -5890,6 +5881,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5911,14 +5911,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{179DDC9E-E391-4AD2-A488-D9C201286EF9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -5926,4 +5918,12 @@
     <ds:schemaRef ds:uri="07db5020-ba8e-48bf-aa17-fbace2a70736"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48999028-4F3E-48D7-8FDD-8CE421B12A65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>